<commit_message>
updates to several models, controllers and the db schema
</commit_message>
<xml_diff>
--- a/config/seeds.xlsx
+++ b/config/seeds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Desktop\code\hotel-worx-3\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39674A30-8FBF-4CD1-B4BE-C9AF119B032A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFE7D99-8E97-4CB2-A516-41CDA67B5DAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="res_rooms (old)" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4020" uniqueCount="2006">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4021" uniqueCount="2007">
   <si>
     <t>room_num</t>
   </si>
@@ -6053,6 +6053,9 @@
   </si>
   <si>
     <t>USA</t>
+  </si>
+  <si>
+    <t>allow_charges</t>
   </si>
 </sst>
 </file>
@@ -16215,11 +16218,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D42255F-FA0E-4B98-904D-E6CC9AC6492A}">
-  <dimension ref="A1:M201"/>
+  <dimension ref="A1:N201"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M201" sqref="M2:M201"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2:N201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16235,10 +16238,11 @@
     <col min="10" max="10" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="147.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="147.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1693</v>
       </c>
@@ -16275,11 +16279,14 @@
       <c r="L1" s="10" t="s">
         <v>1467</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="M1" s="4" t="s">
+        <v>2006</v>
+      </c>
+      <c r="N1" s="22" t="s">
         <v>1248</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1001</v>
       </c>
@@ -16316,12 +16323,15 @@
       <c r="L2" s="11" t="s">
         <v>1478</v>
       </c>
-      <c r="M2" s="11" t="str">
-        <f>"("&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;G2&amp;", "&amp;H2&amp;", "&amp;I2&amp;", '"&amp;J2&amp;"', '"&amp;K2&amp;"', '"&amp;L2&amp;"'),"</f>
-        <v>(1001, 1001, 1, DATE_SUB(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 1, 9, '109.99', '190501001001', 'needs a late checkout time'),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M2" s="6">
+        <v>1</v>
+      </c>
+      <c r="N2" s="11" t="str">
+        <f>"("&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;G2&amp;", "&amp;H2&amp;", "&amp;I2&amp;", '"&amp;J2&amp;"', '"&amp;K2&amp;"', '"&amp;L2&amp;"', "&amp;M2&amp;"),"</f>
+        <v>(1001, 1001, 1, DATE_SUB(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 1, 9, '109.99', '190501001001', 'needs a late checkout time', 1),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1002</v>
       </c>
@@ -16356,12 +16366,15 @@
         <v>1482</v>
       </c>
       <c r="L3" s="11"/>
-      <c r="M3" s="11" t="str">
-        <f t="shared" ref="M3:M66" si="0">"("&amp;A3&amp;", "&amp;B3&amp;", "&amp;C3&amp;", "&amp;D3&amp;", "&amp;E3&amp;", "&amp;F3&amp;", "&amp;G3&amp;", "&amp;H3&amp;", "&amp;I3&amp;", '"&amp;J3&amp;"', '"&amp;K3&amp;"', '"&amp;L3&amp;"'),"</f>
-        <v>(1002, 1002, 2, DATE_SUB(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 2, 4, '119.99', '190503002001', ''),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M3" s="6">
+        <v>1</v>
+      </c>
+      <c r="N3" s="11" t="str">
+        <f t="shared" ref="N3:N66" si="0">"("&amp;A3&amp;", "&amp;B3&amp;", "&amp;C3&amp;", "&amp;D3&amp;", "&amp;E3&amp;", "&amp;F3&amp;", "&amp;G3&amp;", "&amp;H3&amp;", "&amp;I3&amp;", '"&amp;J3&amp;"', '"&amp;K3&amp;"', '"&amp;L3&amp;"', "&amp;M3&amp;"),"</f>
+        <v>(1002, 1002, 2, DATE_SUB(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 2, 4, '119.99', '190503002001', '', 1),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>1003</v>
       </c>
@@ -16396,12 +16409,15 @@
         <v>1483</v>
       </c>
       <c r="L4" s="11"/>
-      <c r="M4" s="11" t="str">
+      <c r="M4" s="6">
+        <v>1</v>
+      </c>
+      <c r="N4" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1003, 1003, 1, DATE_SUB(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 2, 11, '109.99', '190503003001', ''),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1003, 1003, 1, DATE_SUB(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 2, 11, '109.99', '190503003001', '', 1),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>1004</v>
       </c>
@@ -16438,12 +16454,15 @@
       <c r="L5" s="11" t="s">
         <v>1480</v>
       </c>
-      <c r="M5" s="11" t="str">
+      <c r="M5" s="6">
+        <v>1</v>
+      </c>
+      <c r="N5" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1004, 1004, 2, DATE_SUB(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 1, 12, '119.99', '190504004001', 'wants a good view'),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1004, 1004, 2, DATE_SUB(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 1, 12, '119.99', '190504004001', 'wants a good view', 1),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>1005</v>
       </c>
@@ -16478,12 +16497,15 @@
         <v>1485</v>
       </c>
       <c r="L6" s="11"/>
-      <c r="M6" s="11" t="str">
+      <c r="M6" s="6">
+        <v>1</v>
+      </c>
+      <c r="N6" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1005, 1005, 1, DATE_SUB(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 2, 13, '109.99', '190505005001', ''),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1005, 1005, 1, DATE_SUB(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 2, 13, '109.99', '190505005001', '', 1),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>1006</v>
       </c>
@@ -16518,12 +16540,15 @@
         <v>1486</v>
       </c>
       <c r="L7" s="11"/>
-      <c r="M7" s="11" t="str">
+      <c r="M7" s="6">
+        <v>1</v>
+      </c>
+      <c r="N7" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1006, 1006, 3, DATE_SUB(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 1, 0, 1, 6, '129.99', '190508006001', ''),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1006, 1006, 3, DATE_SUB(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 1, 0, 1, 6, '129.99', '190508006001', '', 1),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>1007</v>
       </c>
@@ -16558,12 +16583,15 @@
         <v>1487</v>
       </c>
       <c r="L8" s="11"/>
-      <c r="M8" s="11" t="str">
+      <c r="M8" s="6">
+        <v>1</v>
+      </c>
+      <c r="N8" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1007, 1007, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 2, 23, '109.99', '190509007001', ''),</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1007, 1007, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 2, 23, '109.99', '190509007001', '', 1),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>1008</v>
       </c>
@@ -16598,12 +16626,15 @@
         <v>1488</v>
       </c>
       <c r="L9" s="11"/>
-      <c r="M9" s="11" t="str">
+      <c r="M9" s="6">
+        <v>1</v>
+      </c>
+      <c r="N9" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1008, 1008, 3, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 2, 26, '129.99', '190511008001', ''),</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1008, 1008, 3, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 2, 26, '129.99', '190511008001', '', 1),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>1009</v>
       </c>
@@ -16638,12 +16669,15 @@
         <v>1489</v>
       </c>
       <c r="L10" s="11"/>
-      <c r="M10" s="11" t="str">
+      <c r="M10" s="6">
+        <v>1</v>
+      </c>
+      <c r="N10" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1009, 1009, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 1, 0, 1, 25, '109.99', '190513009001', ''),</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1009, 1009, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 1, 0, 1, 25, '109.99', '190513009001', '', 1),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>1010</v>
       </c>
@@ -16678,12 +16712,15 @@
         <v>1490</v>
       </c>
       <c r="L11" s="11"/>
-      <c r="M11" s="11" t="str">
+      <c r="M11" s="6">
+        <v>1</v>
+      </c>
+      <c r="N11" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1010, 1010, 3, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 3, 28, '129.99', '190515010001', ''),</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1010, 1010, 3, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 3, 28, '129.99', '190515010001', '', 1),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>1011</v>
       </c>
@@ -16718,12 +16755,15 @@
         <v>1491</v>
       </c>
       <c r="L12" s="11"/>
-      <c r="M12" s="11" t="str">
+      <c r="M12" s="6">
+        <v>1</v>
+      </c>
+      <c r="N12" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1011, 1011, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 1, 0, 1, 27, '109.99', '190517011001', ''),</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1011, 1011, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 1, 0, 1, 27, '109.99', '190517011001', '', 1),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>1012</v>
       </c>
@@ -16758,12 +16798,15 @@
         <v>1492</v>
       </c>
       <c r="L13" s="11"/>
-      <c r="M13" s="11" t="str">
+      <c r="M13" s="6">
+        <v>1</v>
+      </c>
+      <c r="N13" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1012, 1012, 2, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 2, 24, '119.99', '190519012001', ''),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1012, 1012, 2, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 2, 24, '119.99', '190519012001', '', 1),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>1013</v>
       </c>
@@ -16798,12 +16841,15 @@
         <v>1493</v>
       </c>
       <c r="L14" s="11"/>
-      <c r="M14" s="11" t="str">
+      <c r="M14" s="6">
+        <v>1</v>
+      </c>
+      <c r="N14" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1013, 1013, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 2, 29, '109.99', '190521013001', ''),</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1013, 1013, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 2, 29, '109.99', '190521013001', '', 1),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>1014</v>
       </c>
@@ -16838,12 +16884,15 @@
         <v>1494</v>
       </c>
       <c r="L15" s="11"/>
-      <c r="M15" s="11" t="str">
+      <c r="M15" s="6">
+        <v>1</v>
+      </c>
+      <c r="N15" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1014, 1014, 2, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 1, 32, '119.99', '190523014001', ''),</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1014, 1014, 2, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 1, 32, '119.99', '190523014001', '', 1),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>1015</v>
       </c>
@@ -16878,12 +16927,15 @@
         <v>1495</v>
       </c>
       <c r="L16" s="11"/>
-      <c r="M16" s="11" t="str">
+      <c r="M16" s="6">
+        <v>1</v>
+      </c>
+      <c r="N16" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1015, 1015, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 3, 31, '109.99', '190525015001', ''),</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1015, 1015, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 3, 31, '109.99', '190525015001', '', 1),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>1016</v>
       </c>
@@ -16918,12 +16970,15 @@
         <v>1496</v>
       </c>
       <c r="L17" s="11"/>
-      <c r="M17" s="11" t="str">
+      <c r="M17" s="6">
+        <v>1</v>
+      </c>
+      <c r="N17" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1016, 1016, 3, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 1, 0, 1, 50, '129.99', '190528016001', ''),</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1016, 1016, 3, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 1, 0, 1, 50, '129.99', '190528016001', '', 1),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>1017</v>
       </c>
@@ -16960,12 +17015,15 @@
       <c r="L18" s="11" t="s">
         <v>1478</v>
       </c>
-      <c r="M18" s="11" t="str">
+      <c r="M18" s="6">
+        <v>1</v>
+      </c>
+      <c r="N18" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1017, 1017, 1, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 2, 63, '109.99', '190529017001', 'needs a late checkout time'),</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1017, 1017, 1, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 2, 63, '109.99', '190529017001', 'needs a late checkout time', 1),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>1018</v>
       </c>
@@ -17000,12 +17058,15 @@
         <v>1498</v>
       </c>
       <c r="L19" s="11"/>
-      <c r="M19" s="11" t="str">
+      <c r="M19" s="6">
+        <v>1</v>
+      </c>
+      <c r="N19" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1018, 1018, 3, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 2, 56, '129.99', '190601018001', ''),</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1018, 1018, 3, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 2, 56, '129.99', '190601018001', '', 1),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>1019</v>
       </c>
@@ -17040,12 +17101,15 @@
         <v>1499</v>
       </c>
       <c r="L20" s="11"/>
-      <c r="M20" s="11" t="str">
+      <c r="M20" s="6">
+        <v>1</v>
+      </c>
+      <c r="N20" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1019, 1019, 1, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 1, 65, '109.99', '190601019001', ''),</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1019, 1019, 1, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 1, 65, '109.99', '190601019001', '', 1),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>1020</v>
       </c>
@@ -17082,12 +17146,15 @@
       <c r="L21" s="11" t="s">
         <v>1480</v>
       </c>
-      <c r="M21" s="11" t="str">
+      <c r="M21" s="6">
+        <v>1</v>
+      </c>
+      <c r="N21" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1020, 1020, 3, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 3, 58, '129.99', '190601020001', 'wants a good view'),</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1020, 1020, 3, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 3, 58, '129.99', '190601020001', 'wants a good view', 1),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>1021</v>
       </c>
@@ -17122,12 +17189,15 @@
         <v>1501</v>
       </c>
       <c r="L22" s="11"/>
-      <c r="M22" s="11" t="str">
+      <c r="M22" s="6">
+        <v>1</v>
+      </c>
+      <c r="N22" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1021, 1021, 1, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 1, 67, '109.99', '190601021001', ''),</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1021, 1021, 1, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 1, 67, '109.99', '190601021001', '', 1),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>1022</v>
       </c>
@@ -17162,12 +17232,15 @@
         <v>1502</v>
       </c>
       <c r="L23" s="11"/>
-      <c r="M23" s="11" t="str">
+      <c r="M23" s="6">
+        <v>1</v>
+      </c>
+      <c r="N23" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1022, 1022, 2, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 1, 0, 2, 62, '119.99', '190601022001', ''),</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1022, 1022, 2, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 1, 0, 2, 62, '119.99', '190601022001', '', 1),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>1023</v>
       </c>
@@ -17202,12 +17275,15 @@
         <v>1503</v>
       </c>
       <c r="L24" s="11"/>
-      <c r="M24" s="11" t="str">
+      <c r="M24" s="6">
+        <v>1</v>
+      </c>
+      <c r="N24" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1023, 1023, 1, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 1, 0, 2, 69, '109.99', '190602023001', ''),</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1023, 1023, 1, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 1, 0, 2, 69, '109.99', '190602023001', '', 1),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>1024</v>
       </c>
@@ -17242,12 +17318,15 @@
         <v>1504</v>
       </c>
       <c r="L25" s="11"/>
-      <c r="M25" s="11" t="str">
+      <c r="M25" s="6">
+        <v>1</v>
+      </c>
+      <c r="N25" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1024, 1024, 2, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 1, 0, 1, 64, '119.99', '190602024001', ''),</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1024, 1024, 2, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 1, 0, 1, 64, '119.99', '190602024001', '', 1),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>1025</v>
       </c>
@@ -17282,12 +17361,15 @@
         <v>1505</v>
       </c>
       <c r="L26" s="11"/>
-      <c r="M26" s="11" t="str">
+      <c r="M26" s="6">
+        <v>1</v>
+      </c>
+      <c r="N26" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1025, 1025, 1, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 3, 71, '109.99', '190602025001', ''),</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1025, 1025, 1, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 3, 71, '109.99', '190602025001', '', 1),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>1026</v>
       </c>
@@ -17324,12 +17406,15 @@
       <c r="L27" s="11" t="s">
         <v>1478</v>
       </c>
-      <c r="M27" s="11" t="str">
+      <c r="M27" s="6">
+        <v>1</v>
+      </c>
+      <c r="N27" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1026, 1026, 3, DATE_SUB(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 1, 8, '129.99', '190603026001', 'needs a late checkout time'),</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1026, 1026, 3, DATE_SUB(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 1, 8, '129.99', '190603026001', 'needs a late checkout time', 1),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>1027</v>
       </c>
@@ -17364,12 +17449,15 @@
         <v>1507</v>
       </c>
       <c r="L28" s="11"/>
-      <c r="M28" s="11" t="str">
+      <c r="M28" s="6">
+        <v>1</v>
+      </c>
+      <c r="N28" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1027, 1027, 1, DATE_SUB(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 2, 15, '109.99', '190603027001', ''),</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1027, 1027, 1, DATE_SUB(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 2, 15, '109.99', '190603027001', '', 1),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>1028</v>
       </c>
@@ -17404,12 +17492,15 @@
         <v>1508</v>
       </c>
       <c r="L29" s="11"/>
-      <c r="M29" s="11" t="str">
+      <c r="M29" s="6">
+        <v>1</v>
+      </c>
+      <c r="N29" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1028, 1028, 3, DATE_SUB(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 1, 0, 2, 10, '129.99', '190603028001', ''),</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1028, 1028, 3, DATE_SUB(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 1, 0, 2, 10, '129.99', '190603028001', '', 1),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>1029</v>
       </c>
@@ -17444,12 +17535,15 @@
         <v>1509</v>
       </c>
       <c r="L30" s="11"/>
-      <c r="M30" s="11" t="str">
+      <c r="M30" s="6">
+        <v>1</v>
+      </c>
+      <c r="N30" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1029, 1029, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 1, 33, '109.99', '190604029001', ''),</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1029, 1029, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 1, 33, '109.99', '190604029001', '', 1),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>1030</v>
       </c>
@@ -17484,12 +17578,15 @@
         <v>1510</v>
       </c>
       <c r="L31" s="11"/>
-      <c r="M31" s="11" t="str">
+      <c r="M31" s="6">
+        <v>1</v>
+      </c>
+      <c r="N31" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1030, 1030, 3, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 3, 30, '129.99', '190604030001', ''),</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1030, 1030, 3, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 3, 30, '129.99', '190604030001', '', 1),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>1031</v>
       </c>
@@ -17524,12 +17621,15 @@
         <v>1511</v>
       </c>
       <c r="L32" s="11"/>
-      <c r="M32" s="11" t="str">
+      <c r="M32" s="6">
+        <v>1</v>
+      </c>
+      <c r="N32" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1031, 1031, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 1, 0, 1, 35, '109.99', '190604031001', ''),</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1031, 1031, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 1, 0, 1, 35, '109.99', '190604031001', '', 1),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>1032</v>
       </c>
@@ -17564,12 +17664,15 @@
         <v>1512</v>
       </c>
       <c r="L33" s="11"/>
-      <c r="M33" s="11" t="str">
+      <c r="M33" s="6">
+        <v>1</v>
+      </c>
+      <c r="N33" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1032, 1032, 2, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 2, 34, '119.99', '190604032001', ''),</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1032, 1032, 2, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 2, 34, '119.99', '190604032001', '', 1),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>1033</v>
       </c>
@@ -17604,12 +17707,15 @@
         <v>1513</v>
       </c>
       <c r="L34" s="11"/>
-      <c r="M34" s="11" t="str">
+      <c r="M34" s="6">
+        <v>1</v>
+      </c>
+      <c r="N34" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1033, 1033, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 1, 0, 2, 37, '109.99', '190605033001', ''),</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1033, 1033, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 1, 0, 2, 37, '109.99', '190605033001', '', 1),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>1034</v>
       </c>
@@ -17644,12 +17750,15 @@
         <v>1514</v>
       </c>
       <c r="L35" s="11"/>
-      <c r="M35" s="11" t="str">
+      <c r="M35" s="6">
+        <v>1</v>
+      </c>
+      <c r="N35" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1034, 1034, 2, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 1, 42, '119.99', '190605034001', ''),</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1034, 1034, 2, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 1, 42, '119.99', '190605034001', '', 1),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>1035</v>
       </c>
@@ -17684,12 +17793,15 @@
         <v>1515</v>
       </c>
       <c r="L36" s="11"/>
-      <c r="M36" s="11" t="str">
+      <c r="M36" s="6">
+        <v>1</v>
+      </c>
+      <c r="N36" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1035, 1035, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 4, 39, '109.99', '190605035001', ''),</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1035, 1035, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 4, 39, '109.99', '190605035001', '', 1),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>1036</v>
       </c>
@@ -17726,12 +17838,15 @@
       <c r="L37" s="11" t="s">
         <v>1478</v>
       </c>
-      <c r="M37" s="11" t="str">
+      <c r="M37" s="6">
+        <v>1</v>
+      </c>
+      <c r="N37" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1036, 1036, 3, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 1, 36, '129.99', '190605036001', 'needs a late checkout time'),</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1036, 1036, 3, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 1, 36, '129.99', '190605036001', 'needs a late checkout time', 1),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>1037</v>
       </c>
@@ -17766,12 +17881,15 @@
         <v>1517</v>
       </c>
       <c r="L38" s="11"/>
-      <c r="M38" s="11" t="str">
+      <c r="M38" s="6">
+        <v>1</v>
+      </c>
+      <c r="N38" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1037, 1037, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 2, 41, '109.99', '190605037001', ''),</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1037, 1037, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 2, 41, '109.99', '190605037001', '', 1),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <v>1038</v>
       </c>
@@ -17806,12 +17924,15 @@
         <v>1518</v>
       </c>
       <c r="L39" s="11"/>
-      <c r="M39" s="11" t="str">
+      <c r="M39" s="6">
+        <v>1</v>
+      </c>
+      <c r="N39" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1038, 1038, 3, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 1, 0, 2, 60, '129.99', '190605038001', ''),</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1038, 1038, 3, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 1, 0, 2, 60, '129.99', '190605038001', '', 1),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <v>1039</v>
       </c>
@@ -17846,12 +17967,15 @@
         <v>1519</v>
       </c>
       <c r="L40" s="11"/>
-      <c r="M40" s="11" t="str">
+      <c r="M40" s="6">
+        <v>1</v>
+      </c>
+      <c r="N40" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1039, 1039, 1, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 1, 73, '109.99', '190605039001', ''),</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1039, 1039, 1, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 1, 0, 1, 73, '109.99', '190605039001', '', 1),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <v>1040</v>
       </c>
@@ -17886,12 +18010,15 @@
         <v>1520</v>
       </c>
       <c r="L41" s="11"/>
-      <c r="M41" s="11" t="str">
+      <c r="M41" s="6">
+        <v>1</v>
+      </c>
+      <c r="N41" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1040, 1040, 3, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 3, 66, '129.99', '190606040001', ''),</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1040, 1040, 3, DATE_SUB(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 1, 0, 3, 66, '129.99', '190606040001', '', 1),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>1041</v>
       </c>
@@ -17928,12 +18055,15 @@
       <c r="L42" s="11" t="s">
         <v>1478</v>
       </c>
-      <c r="M42" s="11" t="str">
+      <c r="M42" s="6">
+        <v>1</v>
+      </c>
+      <c r="N42" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1041, 1041, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 1, null, '109.99', '190606041001', 'needs a late checkout time'),</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1041, 1041, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 1, null, '109.99', '190606041001', 'needs a late checkout time', 1),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>1042</v>
       </c>
@@ -17968,12 +18098,15 @@
         <v>1522</v>
       </c>
       <c r="L43" s="11"/>
-      <c r="M43" s="11" t="str">
+      <c r="M43" s="6">
+        <v>1</v>
+      </c>
+      <c r="N43" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1042, 1042, 2, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 0, 0, 2, null, '119.99', '190607042001', ''),</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1042, 1042, 2, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 0, 0, 2, null, '119.99', '190607042001', '', 1),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>1043</v>
       </c>
@@ -18008,12 +18141,15 @@
         <v>1523</v>
       </c>
       <c r="L44" s="11"/>
-      <c r="M44" s="11" t="str">
+      <c r="M44" s="6">
+        <v>1</v>
+      </c>
+      <c r="N44" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1043, 1043, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 2, null, '109.99', '190607043001', ''),</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1043, 1043, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 2, null, '109.99', '190607043001', '', 1),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>1044</v>
       </c>
@@ -18048,12 +18184,15 @@
         <v>1524</v>
       </c>
       <c r="L45" s="11"/>
-      <c r="M45" s="11" t="str">
+      <c r="M45" s="6">
+        <v>1</v>
+      </c>
+      <c r="N45" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1044, 1044, 2, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 1, null, '119.99', '190607044001', ''),</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1044, 1044, 2, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 1, null, '119.99', '190607044001', '', 1),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>1045</v>
       </c>
@@ -18088,12 +18227,15 @@
         <v>1525</v>
       </c>
       <c r="L46" s="11"/>
-      <c r="M46" s="11" t="str">
+      <c r="M46" s="6">
+        <v>1</v>
+      </c>
+      <c r="N46" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1045, 1045, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 3, null, '109.99', '190607045001', ''),</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1045, 1045, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 3, null, '109.99', '190607045001', '', 1),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <v>1046</v>
       </c>
@@ -18128,12 +18270,15 @@
         <v>1526</v>
       </c>
       <c r="L47" s="11"/>
-      <c r="M47" s="11" t="str">
+      <c r="M47" s="6">
+        <v>1</v>
+      </c>
+      <c r="N47" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1046, 1046, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 1, null, '129.99', '190607046001', ''),</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1046, 1046, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 1, null, '129.99', '190607046001', '', 1),</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <v>1047</v>
       </c>
@@ -18170,12 +18315,15 @@
       <c r="L48" s="11" t="s">
         <v>1478</v>
       </c>
-      <c r="M48" s="11" t="str">
+      <c r="M48" s="6">
+        <v>1</v>
+      </c>
+      <c r="N48" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1047, 1047, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 2, null, '109.99', '190608047001', 'needs a late checkout time'),</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1047, 1047, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 2, null, '109.99', '190608047001', 'needs a late checkout time', 1),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <v>1048</v>
       </c>
@@ -18210,12 +18358,15 @@
         <v>1528</v>
       </c>
       <c r="L49" s="11"/>
-      <c r="M49" s="11" t="str">
+      <c r="M49" s="6">
+        <v>1</v>
+      </c>
+      <c r="N49" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1048, 1048, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 2, null, '129.99', '190608048001', ''),</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1048, 1048, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 2, null, '129.99', '190608048001', '', 1),</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>1049</v>
       </c>
@@ -18250,12 +18401,15 @@
         <v>1529</v>
       </c>
       <c r="L50" s="11"/>
-      <c r="M50" s="11" t="str">
+      <c r="M50" s="6">
+        <v>1</v>
+      </c>
+      <c r="N50" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1049, 1049, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 1, null, '109.99', '190608049001', ''),</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1049, 1049, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 1, null, '109.99', '190608049001', '', 1),</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>1050</v>
       </c>
@@ -18290,12 +18444,15 @@
         <v>1530</v>
       </c>
       <c r="L51" s="11"/>
-      <c r="M51" s="11" t="str">
+      <c r="M51" s="6">
+        <v>1</v>
+      </c>
+      <c r="N51" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1050, 1050, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 3, null, '129.99', '190608050001', ''),</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1050, 1050, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 3, null, '129.99', '190608050001', '', 1),</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <v>1051</v>
       </c>
@@ -18330,12 +18487,15 @@
         <v>1531</v>
       </c>
       <c r="L52" s="11"/>
-      <c r="M52" s="11" t="str">
+      <c r="M52" s="6">
+        <v>1</v>
+      </c>
+      <c r="N52" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1051, 1051, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 0, 0, 1, null, '109.99', '190608051001', ''),</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1051, 1051, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 0, 0, 1, null, '109.99', '190608051001', '', 1),</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
         <v>1052</v>
       </c>
@@ -18370,12 +18530,15 @@
         <v>1532</v>
       </c>
       <c r="L53" s="11"/>
-      <c r="M53" s="11" t="str">
+      <c r="M53" s="6">
+        <v>1</v>
+      </c>
+      <c r="N53" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1052, 1052, 2, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 2, null, '119.99', '190608052001', ''),</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1052, 1052, 2, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 2, null, '119.99', '190608052001', '', 1),</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <v>1053</v>
       </c>
@@ -18410,12 +18573,15 @@
         <v>1533</v>
       </c>
       <c r="L54" s="11"/>
-      <c r="M54" s="11" t="str">
+      <c r="M54" s="6">
+        <v>1</v>
+      </c>
+      <c r="N54" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1053, 1053, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 2, null, '109.99', '190609053001', ''),</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1053, 1053, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 2, null, '109.99', '190609053001', '', 1),</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <v>1054</v>
       </c>
@@ -18450,12 +18616,15 @@
         <v>1534</v>
       </c>
       <c r="L55" s="11"/>
-      <c r="M55" s="11" t="str">
+      <c r="M55" s="6">
+        <v>1</v>
+      </c>
+      <c r="N55" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1054, 1054, 2, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 0, 0, 1, null, '119.99', '190609054001', ''),</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1054, 1054, 2, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 0, 0, 1, null, '119.99', '190609054001', '', 1),</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
         <v>1055</v>
       </c>
@@ -18490,12 +18659,15 @@
         <v>1535</v>
       </c>
       <c r="L56" s="11"/>
-      <c r="M56" s="11" t="str">
+      <c r="M56" s="6">
+        <v>1</v>
+      </c>
+      <c r="N56" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1055, 1055, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 3, null, '109.99', '190609055001', ''),</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1055, 1055, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 3, null, '109.99', '190609055001', '', 1),</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="6">
         <v>1056</v>
       </c>
@@ -18530,12 +18702,15 @@
         <v>1536</v>
       </c>
       <c r="L57" s="11"/>
-      <c r="M57" s="11" t="str">
+      <c r="M57" s="6">
+        <v>1</v>
+      </c>
+      <c r="N57" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1056, 1056, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 1, null, '129.99', '190609056001', ''),</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1056, 1056, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 1, null, '129.99', '190609056001', '', 1),</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="6">
         <v>1057</v>
       </c>
@@ -18570,12 +18745,15 @@
         <v>1537</v>
       </c>
       <c r="L58" s="11"/>
-      <c r="M58" s="11" t="str">
+      <c r="M58" s="6">
+        <v>1</v>
+      </c>
+      <c r="N58" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1057, 1057, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 2, null, '109.99', '190609057001', ''),</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1057, 1057, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 2, null, '109.99', '190609057001', '', 1),</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
         <v>1058</v>
       </c>
@@ -18610,12 +18788,15 @@
         <v>1538</v>
       </c>
       <c r="L59" s="11"/>
-      <c r="M59" s="11" t="str">
+      <c r="M59" s="6">
+        <v>1</v>
+      </c>
+      <c r="N59" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1058, 1058, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 2, null, '129.99', '190610058001', ''),</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1058, 1058, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 2, null, '129.99', '190610058001', '', 1),</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="6">
         <v>1059</v>
       </c>
@@ -18650,12 +18831,15 @@
         <v>1539</v>
       </c>
       <c r="L60" s="11"/>
-      <c r="M60" s="11" t="str">
+      <c r="M60" s="6">
+        <v>1</v>
+      </c>
+      <c r="N60" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1059, 1059, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 1, null, '109.99', '190610059001', ''),</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1059, 1059, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 1, null, '109.99', '190610059001', '', 1),</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
         <v>1060</v>
       </c>
@@ -18690,12 +18874,15 @@
         <v>1540</v>
       </c>
       <c r="L61" s="11"/>
-      <c r="M61" s="11" t="str">
+      <c r="M61" s="6">
+        <v>1</v>
+      </c>
+      <c r="N61" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1060, 1060, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 0, 0, 3, null, '129.99', '190610060001', ''),</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1060, 1060, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 0, 0, 3, null, '129.99', '190610060001', '', 1),</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="6">
         <v>1061</v>
       </c>
@@ -18732,12 +18919,15 @@
       <c r="L62" s="11" t="s">
         <v>1478</v>
       </c>
-      <c r="M62" s="11" t="str">
+      <c r="M62" s="6">
+        <v>1</v>
+      </c>
+      <c r="N62" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1061, 1061, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 1, null, '109.99', '190610061001', 'needs a late checkout time'),</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1061, 1061, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 1, null, '109.99', '190610061001', 'needs a late checkout time', 1),</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="6">
         <v>1062</v>
       </c>
@@ -18772,12 +18962,15 @@
         <v>1542</v>
       </c>
       <c r="L63" s="11"/>
-      <c r="M63" s="11" t="str">
+      <c r="M63" s="6">
+        <v>1</v>
+      </c>
+      <c r="N63" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1062, 1062, 2, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 2, null, '119.99', '190611062001', ''),</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1062, 1062, 2, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 2, null, '119.99', '190611062001', '', 1),</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" s="6">
         <v>1063</v>
       </c>
@@ -18812,12 +19005,15 @@
         <v>1543</v>
       </c>
       <c r="L64" s="11"/>
-      <c r="M64" s="11" t="str">
+      <c r="M64" s="6">
+        <v>1</v>
+      </c>
+      <c r="N64" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1063, 1063, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 2, null, '109.99', '190611063001', ''),</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1063, 1063, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 2, null, '109.99', '190611063001', '', 1),</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" s="6">
         <v>1064</v>
       </c>
@@ -18852,12 +19048,15 @@
         <v>1544</v>
       </c>
       <c r="L65" s="11"/>
-      <c r="M65" s="11" t="str">
+      <c r="M65" s="6">
+        <v>1</v>
+      </c>
+      <c r="N65" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1064, 1064, 2, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 1, null, '119.99', '190612064001', ''),</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1064, 1064, 2, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 1, null, '119.99', '190612064001', '', 1),</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" s="6">
         <v>1065</v>
       </c>
@@ -18894,12 +19093,15 @@
       <c r="L66" s="11" t="s">
         <v>1479</v>
       </c>
-      <c r="M66" s="11" t="str">
+      <c r="M66" s="6">
+        <v>1</v>
+      </c>
+      <c r="N66" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>(1065, 1065, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 3, null, '109.99', '190612065001', 'wants a large screen tv'),</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1065, 1065, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 3, null, '109.99', '190612065001', 'wants a large screen tv', 1),</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" s="6">
         <v>1066</v>
       </c>
@@ -18934,12 +19136,15 @@
         <v>1546</v>
       </c>
       <c r="L67" s="11"/>
-      <c r="M67" s="11" t="str">
-        <f t="shared" ref="M67:M130" si="1">"("&amp;A67&amp;", "&amp;B67&amp;", "&amp;C67&amp;", "&amp;D67&amp;", "&amp;E67&amp;", "&amp;F67&amp;", "&amp;G67&amp;", "&amp;H67&amp;", "&amp;I67&amp;", '"&amp;J67&amp;"', '"&amp;K67&amp;"', '"&amp;L67&amp;"'),"</f>
-        <v>(1066, 1066, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 0, 0, 1, null, '129.99', '190613066001', ''),</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M67" s="6">
+        <v>1</v>
+      </c>
+      <c r="N67" s="11" t="str">
+        <f t="shared" ref="N67:N130" si="1">"("&amp;A67&amp;", "&amp;B67&amp;", "&amp;C67&amp;", "&amp;D67&amp;", "&amp;E67&amp;", "&amp;F67&amp;", "&amp;G67&amp;", "&amp;H67&amp;", "&amp;I67&amp;", '"&amp;J67&amp;"', '"&amp;K67&amp;"', '"&amp;L67&amp;"', "&amp;M67&amp;"),"</f>
+        <v>(1066, 1066, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 0, 0, 1, null, '129.99', '190613066001', '', 1),</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" s="6">
         <v>1067</v>
       </c>
@@ -18974,12 +19179,15 @@
         <v>1547</v>
       </c>
       <c r="L68" s="11"/>
-      <c r="M68" s="11" t="str">
+      <c r="M68" s="6">
+        <v>1</v>
+      </c>
+      <c r="N68" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1067, 1067, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 2, null, '109.99', '190613067001', ''),</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1067, 1067, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 2, null, '109.99', '190613067001', '', 1),</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" s="6">
         <v>1068</v>
       </c>
@@ -19014,12 +19222,15 @@
         <v>1548</v>
       </c>
       <c r="L69" s="11"/>
-      <c r="M69" s="11" t="str">
+      <c r="M69" s="6">
+        <v>1</v>
+      </c>
+      <c r="N69" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1068, 1068, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 2, null, '129.99', '190613068001', ''),</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1068, 1068, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 2, null, '129.99', '190613068001', '', 1),</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" s="6">
         <v>1069</v>
       </c>
@@ -19054,12 +19265,15 @@
         <v>1549</v>
       </c>
       <c r="L70" s="11"/>
-      <c r="M70" s="11" t="str">
+      <c r="M70" s="6">
+        <v>1</v>
+      </c>
+      <c r="N70" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1069, 1069, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 1, null, '109.99', '190613069001', ''),</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1069, 1069, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 1, null, '109.99', '190613069001', '', 1),</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" s="6">
         <v>1070</v>
       </c>
@@ -19094,12 +19308,15 @@
         <v>1550</v>
       </c>
       <c r="L71" s="11"/>
-      <c r="M71" s="11" t="str">
+      <c r="M71" s="6">
+        <v>1</v>
+      </c>
+      <c r="N71" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1070, 1070, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 3, null, '129.99', '190614070001', ''),</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1070, 1070, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 3, null, '129.99', '190614070001', '', 1),</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" s="6">
         <v>1071</v>
       </c>
@@ -19134,12 +19351,15 @@
         <v>1551</v>
       </c>
       <c r="L72" s="11"/>
-      <c r="M72" s="11" t="str">
+      <c r="M72" s="6">
+        <v>1</v>
+      </c>
+      <c r="N72" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1071, 1071, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 10 DAY), 0, 0, 1, null, '109.99', '190614071001', ''),</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1071, 1071, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 10 DAY), 0, 0, 1, null, '109.99', '190614071001', '', 1),</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" s="6">
         <v>1072</v>
       </c>
@@ -19174,12 +19394,15 @@
         <v>1552</v>
       </c>
       <c r="L73" s="11"/>
-      <c r="M73" s="11" t="str">
+      <c r="M73" s="6">
+        <v>1</v>
+      </c>
+      <c r="N73" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1072, 1072, 2, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 0, 0, 2, null, '119.99', '190614072001', ''),</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1072, 1072, 2, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 0, 0, 2, null, '119.99', '190614072001', '', 1),</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" s="6">
         <v>1073</v>
       </c>
@@ -19216,12 +19439,15 @@
       <c r="L74" s="11" t="s">
         <v>1478</v>
       </c>
-      <c r="M74" s="11" t="str">
+      <c r="M74" s="6">
+        <v>1</v>
+      </c>
+      <c r="N74" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1073, 1073, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 2, null, '109.99', '190615073001', 'needs a late checkout time'),</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1073, 1073, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 2, null, '109.99', '190615073001', 'needs a late checkout time', 1),</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" s="6">
         <v>1074</v>
       </c>
@@ -19256,12 +19482,15 @@
         <v>1554</v>
       </c>
       <c r="L75" s="11"/>
-      <c r="M75" s="11" t="str">
+      <c r="M75" s="6">
+        <v>1</v>
+      </c>
+      <c r="N75" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1074, 1074, 2, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 1, null, '119.99', '190615074001', ''),</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1074, 1074, 2, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 1, null, '119.99', '190615074001', '', 1),</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" s="6">
         <v>1075</v>
       </c>
@@ -19296,12 +19525,15 @@
         <v>1555</v>
       </c>
       <c r="L76" s="11"/>
-      <c r="M76" s="11" t="str">
+      <c r="M76" s="6">
+        <v>1</v>
+      </c>
+      <c r="N76" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1075, 1075, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 3, null, '109.99', '190615075001', ''),</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1075, 1075, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 3, null, '109.99', '190615075001', '', 1),</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" s="6">
         <v>1076</v>
       </c>
@@ -19336,12 +19568,15 @@
         <v>1556</v>
       </c>
       <c r="L77" s="11"/>
-      <c r="M77" s="11" t="str">
+      <c r="M77" s="6">
+        <v>1</v>
+      </c>
+      <c r="N77" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1076, 1076, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 1, null, '129.99', '190615076001', ''),</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1076, 1076, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 1, null, '129.99', '190615076001', '', 1),</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" s="6">
         <v>1077</v>
       </c>
@@ -19376,12 +19611,15 @@
         <v>1557</v>
       </c>
       <c r="L78" s="11"/>
-      <c r="M78" s="11" t="str">
+      <c r="M78" s="6">
+        <v>1</v>
+      </c>
+      <c r="N78" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1077, 1077, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 2, null, '109.99', '190615077001', ''),</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1077, 1077, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 2, null, '109.99', '190615077001', '', 1),</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" s="6">
         <v>1078</v>
       </c>
@@ -19416,12 +19654,15 @@
         <v>1558</v>
       </c>
       <c r="L79" s="11"/>
-      <c r="M79" s="11" t="str">
+      <c r="M79" s="6">
+        <v>1</v>
+      </c>
+      <c r="N79" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1078, 1078, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 0, 0, 2, null, '129.99', '190616078001', ''),</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1078, 1078, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 0, 0, 2, null, '129.99', '190616078001', '', 1),</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" s="6">
         <v>1079</v>
       </c>
@@ -19456,12 +19697,15 @@
         <v>1559</v>
       </c>
       <c r="L80" s="11"/>
-      <c r="M80" s="11" t="str">
+      <c r="M80" s="6">
+        <v>1</v>
+      </c>
+      <c r="N80" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1079, 1079, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 1, null, '109.99', '190616079001', ''),</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1079, 1079, 1, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 1 DAY), 0, 0, 1, null, '109.99', '190616079001', '', 1),</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" s="6">
         <v>1080</v>
       </c>
@@ -19496,12 +19740,15 @@
         <v>1560</v>
       </c>
       <c r="L81" s="11"/>
-      <c r="M81" s="11" t="str">
+      <c r="M81" s="6">
+        <v>1</v>
+      </c>
+      <c r="N81" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1080, 1080, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 3, null, '129.99', '190616080001', ''),</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1080, 1080, 3, CURDATE(), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 3, null, '129.99', '190616080001', '', 1),</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" s="6">
         <v>1081</v>
       </c>
@@ -19536,12 +19783,15 @@
         <v>1561</v>
       </c>
       <c r="L82" s="11"/>
-      <c r="M82" s="11" t="str">
+      <c r="M82" s="6">
+        <v>1</v>
+      </c>
+      <c r="N82" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1081, 1081, 1, DATE_SUB(CURDATE(), INTERVAL 3 DAY), CURDATE(), 1, 0, 1, 17, '109.99', '190616081001', ''),</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1081, 1081, 1, DATE_SUB(CURDATE(), INTERVAL 3 DAY), CURDATE(), 1, 0, 1, 17, '109.99', '190616081001', '', 1),</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" s="6">
         <v>1082</v>
       </c>
@@ -19576,12 +19826,15 @@
         <v>1562</v>
       </c>
       <c r="L83" s="11"/>
-      <c r="M83" s="11" t="str">
+      <c r="M83" s="6">
+        <v>1</v>
+      </c>
+      <c r="N83" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1082, 1082, 2, DATE_SUB(CURDATE(), INTERVAL 3 DAY), CURDATE(), 1, 0, 2, 14, '119.99', '190617082001', ''),</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1082, 1082, 2, DATE_SUB(CURDATE(), INTERVAL 3 DAY), CURDATE(), 1, 0, 2, 14, '119.99', '190617082001', '', 1),</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" s="6">
         <v>1083</v>
       </c>
@@ -19618,12 +19871,15 @@
       <c r="L84" s="11" t="s">
         <v>1478</v>
       </c>
-      <c r="M84" s="11" t="str">
+      <c r="M84" s="6">
+        <v>1</v>
+      </c>
+      <c r="N84" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1083, 1083, 1, DATE_SUB(CURDATE(), INTERVAL 3 DAY), CURDATE(), 1, 0, 2, 19, '109.99', '190617083001', 'needs a late checkout time'),</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1083, 1083, 1, DATE_SUB(CURDATE(), INTERVAL 3 DAY), CURDATE(), 1, 0, 2, 19, '109.99', '190617083001', 'needs a late checkout time', 1),</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85" s="6">
         <v>1084</v>
       </c>
@@ -19658,12 +19914,15 @@
         <v>1564</v>
       </c>
       <c r="L85" s="11"/>
-      <c r="M85" s="11" t="str">
+      <c r="M85" s="6">
+        <v>1</v>
+      </c>
+      <c r="N85" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1084, 1084, 2, DATE_SUB(CURDATE(), INTERVAL 3 DAY), CURDATE(), 1, 0, 1, 22, '119.99', '190617084001', ''),</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1084, 1084, 2, DATE_SUB(CURDATE(), INTERVAL 3 DAY), CURDATE(), 1, 0, 1, 22, '119.99', '190617084001', '', 1),</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86" s="6">
         <v>1085</v>
       </c>
@@ -19698,12 +19957,15 @@
         <v>1565</v>
       </c>
       <c r="L86" s="11"/>
-      <c r="M86" s="11" t="str">
+      <c r="M86" s="6">
+        <v>1</v>
+      </c>
+      <c r="N86" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1085, 1085, 1, DATE_SUB(CURDATE(), INTERVAL 4 DAY), CURDATE(), 1, 0, 3, 3, '109.99', '190617085001', ''),</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1085, 1085, 1, DATE_SUB(CURDATE(), INTERVAL 4 DAY), CURDATE(), 1, 0, 3, 3, '109.99', '190617085001', '', 1),</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87" s="6">
         <v>1086</v>
       </c>
@@ -19738,12 +20000,15 @@
         <v>1566</v>
       </c>
       <c r="L87" s="11"/>
-      <c r="M87" s="11" t="str">
+      <c r="M87" s="6">
+        <v>1</v>
+      </c>
+      <c r="N87" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1086, 1086, 3, DATE_SUB(CURDATE(), INTERVAL 3 DAY), CURDATE(), 1, 0, 4, 16, '129.99', '190618086001', ''),</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1086, 1086, 3, DATE_SUB(CURDATE(), INTERVAL 3 DAY), CURDATE(), 1, 0, 4, 16, '129.99', '190618086001', '', 1),</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88" s="6">
         <v>1087</v>
       </c>
@@ -19778,12 +20043,15 @@
         <v>1567</v>
       </c>
       <c r="L88" s="11"/>
-      <c r="M88" s="11" t="str">
+      <c r="M88" s="6">
+        <v>1</v>
+      </c>
+      <c r="N88" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1087, 1087, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 2, 43, '109.99', '190618087001', ''),</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1087, 1087, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 2, 43, '109.99', '190618087001', '', 1),</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89" s="6">
         <v>1088</v>
       </c>
@@ -19820,12 +20088,15 @@
       <c r="L89" s="11" t="s">
         <v>1480</v>
       </c>
-      <c r="M89" s="11" t="str">
+      <c r="M89" s="6">
+        <v>1</v>
+      </c>
+      <c r="N89" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1088, 1088, 3, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 2, 38, '129.99', '190618088001', 'wants a good view'),</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1088, 1088, 3, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 2, 38, '129.99', '190618088001', 'wants a good view', 1),</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" s="6">
         <v>1089</v>
       </c>
@@ -19860,12 +20131,15 @@
         <v>1569</v>
       </c>
       <c r="L90" s="11"/>
-      <c r="M90" s="11" t="str">
+      <c r="M90" s="6">
+        <v>1</v>
+      </c>
+      <c r="N90" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1089, 1089, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 1, 45, '109.99', '190618089001', ''),</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1089, 1089, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 1, 45, '109.99', '190618089001', '', 1),</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91" s="6">
         <v>1090</v>
       </c>
@@ -19900,12 +20174,15 @@
         <v>1570</v>
       </c>
       <c r="L91" s="11"/>
-      <c r="M91" s="11" t="str">
+      <c r="M91" s="6">
+        <v>1</v>
+      </c>
+      <c r="N91" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1090, 1090, 3, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 3, 40, '129.99', '190619090001', ''),</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1090, 1090, 3, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 3, 40, '129.99', '190619090001', '', 1),</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92" s="6">
         <v>1091</v>
       </c>
@@ -19940,12 +20217,15 @@
         <v>1571</v>
       </c>
       <c r="L92" s="11"/>
-      <c r="M92" s="11" t="str">
+      <c r="M92" s="6">
+        <v>1</v>
+      </c>
+      <c r="N92" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1091, 1091, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 1, 47, '109.99', '190619091001', ''),</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1091, 1091, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 1, 47, '109.99', '190619091001', '', 1),</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93" s="6">
         <v>1092</v>
       </c>
@@ -19980,12 +20260,15 @@
         <v>1572</v>
       </c>
       <c r="L93" s="11"/>
-      <c r="M93" s="11" t="str">
+      <c r="M93" s="6">
+        <v>1</v>
+      </c>
+      <c r="N93" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1092, 1092, 2, DATE_SUB(CURDATE(), INTERVAL 6 DAY), CURDATE(), 1, 0, 2, 2, '119.99', '190619092001', ''),</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1092, 1092, 2, DATE_SUB(CURDATE(), INTERVAL 6 DAY), CURDATE(), 1, 0, 2, 2, '119.99', '190619092001', '', 1),</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94" s="6">
         <v>1093</v>
       </c>
@@ -20020,12 +20303,15 @@
         <v>1573</v>
       </c>
       <c r="L94" s="11"/>
-      <c r="M94" s="11" t="str">
+      <c r="M94" s="6">
+        <v>1</v>
+      </c>
+      <c r="N94" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1093, 1093, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 2, 49, '109.99', '190619093001', ''),</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1093, 1093, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 2, 49, '109.99', '190619093001', '', 1),</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95" s="6">
         <v>1094</v>
       </c>
@@ -20060,12 +20346,15 @@
         <v>1574</v>
       </c>
       <c r="L95" s="11"/>
-      <c r="M95" s="11" t="str">
+      <c r="M95" s="6">
+        <v>1</v>
+      </c>
+      <c r="N95" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1094, 1094, 2, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 1, 44, '119.99', '190619094001', ''),</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1094, 1094, 2, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 1, 44, '119.99', '190619094001', '', 1),</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96" s="6">
         <v>1095</v>
       </c>
@@ -20100,12 +20389,15 @@
         <v>1575</v>
       </c>
       <c r="L96" s="11"/>
-      <c r="M96" s="11" t="str">
+      <c r="M96" s="6">
+        <v>1</v>
+      </c>
+      <c r="N96" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1095, 1095, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 3, 51, '109.99', '190619095001', ''),</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1095, 1095, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 3, 51, '109.99', '190619095001', '', 1),</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A97" s="6">
         <v>1096</v>
       </c>
@@ -20140,12 +20432,15 @@
         <v>1576</v>
       </c>
       <c r="L97" s="11"/>
-      <c r="M97" s="11" t="str">
+      <c r="M97" s="6">
+        <v>1</v>
+      </c>
+      <c r="N97" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1096, 1096, 3, DATE_SUB(CURDATE(), INTERVAL 1 DAY), CURDATE(), 1, 0, 3, 68, '129.99', '190619096001', ''),</v>
-      </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1096, 1096, 3, DATE_SUB(CURDATE(), INTERVAL 1 DAY), CURDATE(), 1, 0, 3, 68, '129.99', '190619096001', '', 1),</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98" s="6">
         <v>1097</v>
       </c>
@@ -20180,12 +20475,15 @@
         <v>1577</v>
       </c>
       <c r="L98" s="11"/>
-      <c r="M98" s="11" t="str">
+      <c r="M98" s="6">
+        <v>1</v>
+      </c>
+      <c r="N98" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1097, 1097, 1, DATE_SUB(CURDATE(), INTERVAL 4 DAY), CURDATE(), 1, 0, 2, 5, '109.99', '190620097001', ''),</v>
-      </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1097, 1097, 1, DATE_SUB(CURDATE(), INTERVAL 4 DAY), CURDATE(), 1, 0, 2, 5, '109.99', '190620097001', '', 1),</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A99" s="6">
         <v>1098</v>
       </c>
@@ -20220,12 +20518,15 @@
         <v>1578</v>
       </c>
       <c r="L99" s="11"/>
-      <c r="M99" s="11" t="str">
+      <c r="M99" s="6">
+        <v>1</v>
+      </c>
+      <c r="N99" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1098, 1098, 3, DATE_SUB(CURDATE(), INTERVAL 1 DAY), CURDATE(), 1, 0, 2, 70, '129.99', '190620098001', ''),</v>
-      </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1098, 1098, 3, DATE_SUB(CURDATE(), INTERVAL 1 DAY), CURDATE(), 1, 0, 2, 70, '129.99', '190620098001', '', 1),</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A100" s="6">
         <v>1099</v>
       </c>
@@ -20262,12 +20563,15 @@
       <c r="L100" s="11" t="s">
         <v>1478</v>
       </c>
-      <c r="M100" s="11" t="str">
+      <c r="M100" s="6">
+        <v>1</v>
+      </c>
+      <c r="N100" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1099, 1099, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 1, 53, '109.99', '190620099001', 'needs a late checkout time'),</v>
-      </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1099, 1099, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 1, 53, '109.99', '190620099001', 'needs a late checkout time', 1),</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A101" s="6">
         <v>1100</v>
       </c>
@@ -20302,12 +20606,15 @@
         <v>1580</v>
       </c>
       <c r="L101" s="11"/>
-      <c r="M101" s="11" t="str">
+      <c r="M101" s="6">
+        <v>1</v>
+      </c>
+      <c r="N101" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1100, 1100, 3, DATE_SUB(CURDATE(), INTERVAL 1 DAY), CURDATE(), 1, 0, 3, 76, '129.99', '190620100001', ''),</v>
-      </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1100, 1100, 3, DATE_SUB(CURDATE(), INTERVAL 1 DAY), CURDATE(), 1, 0, 3, 76, '129.99', '190620100001', '', 1),</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A102" s="6">
         <v>1101</v>
       </c>
@@ -20342,12 +20649,15 @@
         <v>1581</v>
       </c>
       <c r="L102" s="11"/>
-      <c r="M102" s="11" t="str">
+      <c r="M102" s="6">
+        <v>1</v>
+      </c>
+      <c r="N102" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1101, 1101, 1, DATE_SUB(CURDATE(), INTERVAL 6 DAY), CURDATE(), 1, 0, 1, 1, '109.99', '190621101001', ''),</v>
-      </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1101, 1101, 1, DATE_SUB(CURDATE(), INTERVAL 6 DAY), CURDATE(), 1, 0, 1, 1, '109.99', '190621101001', '', 1),</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A103" s="6">
         <v>1102</v>
       </c>
@@ -20382,12 +20692,15 @@
         <v>1582</v>
       </c>
       <c r="L103" s="11"/>
-      <c r="M103" s="11" t="str">
+      <c r="M103" s="6">
+        <v>1</v>
+      </c>
+      <c r="N103" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1102, 1102, 2, DATE_SUB(CURDATE(), INTERVAL 1 DAY), CURDATE(), 1, 0, 2, 72, '119.99', '190621102001', ''),</v>
-      </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1102, 1102, 2, DATE_SUB(CURDATE(), INTERVAL 1 DAY), CURDATE(), 1, 0, 2, 72, '119.99', '190621102001', '', 1),</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A104" s="6">
         <v>1103</v>
       </c>
@@ -20422,12 +20735,15 @@
         <v>1583</v>
       </c>
       <c r="L104" s="11"/>
-      <c r="M104" s="11" t="str">
+      <c r="M104" s="6">
+        <v>1</v>
+      </c>
+      <c r="N104" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1103, 1103, 1, DATE_SUB(CURDATE(), INTERVAL 1 DAY), CURDATE(), 1, 0, 2, 75, '109.99', '190621103001', ''),</v>
-      </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1103, 1103, 1, DATE_SUB(CURDATE(), INTERVAL 1 DAY), CURDATE(), 1, 0, 2, 75, '109.99', '190621103001', '', 1),</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A105" s="6">
         <v>1104</v>
       </c>
@@ -20462,12 +20778,15 @@
         <v>1584</v>
       </c>
       <c r="L105" s="11"/>
-      <c r="M105" s="11" t="str">
+      <c r="M105" s="6">
+        <v>1</v>
+      </c>
+      <c r="N105" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1104, 1104, 2, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 1, 52, '119.99', '190621104001', ''),</v>
-      </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1104, 1104, 2, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 1, 52, '119.99', '190621104001', '', 1),</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A106" s="6">
         <v>1105</v>
       </c>
@@ -20502,12 +20821,15 @@
         <v>1585</v>
       </c>
       <c r="L106" s="11"/>
-      <c r="M106" s="11" t="str">
+      <c r="M106" s="6">
+        <v>1</v>
+      </c>
+      <c r="N106" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1105, 1105, 1, DATE_SUB(CURDATE(), INTERVAL 1 DAY), CURDATE(), 1, 0, 3, 77, '109.99', '190622105001', ''),</v>
-      </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1105, 1105, 1, DATE_SUB(CURDATE(), INTERVAL 1 DAY), CURDATE(), 1, 0, 3, 77, '109.99', '190622105001', '', 1),</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A107" s="6">
         <v>1106</v>
       </c>
@@ -20542,12 +20864,15 @@
         <v>1586</v>
       </c>
       <c r="L107" s="11"/>
-      <c r="M107" s="11" t="str">
+      <c r="M107" s="6">
+        <v>1</v>
+      </c>
+      <c r="N107" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1106, 1106, 3, DATE_SUB(CURDATE(), INTERVAL 3 DAY), CURDATE(), 1, 0, 2, 18, '129.99', '190622106001', ''),</v>
-      </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1106, 1106, 3, DATE_SUB(CURDATE(), INTERVAL 3 DAY), CURDATE(), 1, 0, 2, 18, '129.99', '190622106001', '', 1),</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A108" s="6">
         <v>1107</v>
       </c>
@@ -20582,12 +20907,15 @@
         <v>1587</v>
       </c>
       <c r="L108" s="11"/>
-      <c r="M108" s="11" t="str">
+      <c r="M108" s="6">
+        <v>1</v>
+      </c>
+      <c r="N108" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1107, 1107, 1, DATE_SUB(CURDATE(), INTERVAL 3 DAY), CURDATE(), 1, 0, 2, 21, '109.99', '190623107001', ''),</v>
-      </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1107, 1107, 1, DATE_SUB(CURDATE(), INTERVAL 3 DAY), CURDATE(), 1, 0, 2, 21, '109.99', '190623107001', '', 1),</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A109" s="6">
         <v>1108</v>
       </c>
@@ -20622,12 +20950,15 @@
         <v>1588</v>
       </c>
       <c r="L109" s="11"/>
-      <c r="M109" s="11" t="str">
+      <c r="M109" s="6">
+        <v>1</v>
+      </c>
+      <c r="N109" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1108, 1108, 3, DATE_SUB(CURDATE(), INTERVAL 3 DAY), CURDATE(), 1, 0, 2, 20, '129.99', '190623108001', ''),</v>
-      </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1108, 1108, 3, DATE_SUB(CURDATE(), INTERVAL 3 DAY), CURDATE(), 1, 0, 2, 20, '129.99', '190623108001', '', 1),</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A110" s="6">
         <v>1109</v>
       </c>
@@ -20664,12 +20995,15 @@
       <c r="L110" s="11" t="s">
         <v>1478</v>
       </c>
-      <c r="M110" s="11" t="str">
+      <c r="M110" s="6">
+        <v>1</v>
+      </c>
+      <c r="N110" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1109, 1109, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 1, 55, '109.99', '190623109001', 'needs a late checkout time'),</v>
-      </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1109, 1109, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 1, 55, '109.99', '190623109001', 'needs a late checkout time', 1),</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A111" s="6">
         <v>1110</v>
       </c>
@@ -20704,12 +21038,15 @@
         <v>1590</v>
       </c>
       <c r="L111" s="11"/>
-      <c r="M111" s="11" t="str">
+      <c r="M111" s="6">
+        <v>1</v>
+      </c>
+      <c r="N111" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1110, 1110, 3, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 3, 46, '129.99', '190623110001', ''),</v>
-      </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1110, 1110, 3, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 3, 46, '129.99', '190623110001', '', 1),</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A112" s="6">
         <v>1111</v>
       </c>
@@ -20744,12 +21081,15 @@
         <v>1591</v>
       </c>
       <c r="L112" s="11"/>
-      <c r="M112" s="11" t="str">
+      <c r="M112" s="6">
+        <v>1</v>
+      </c>
+      <c r="N112" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1111, 1111, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 1, 57, '109.99', '190624111001', ''),</v>
-      </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1111, 1111, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 1, 57, '109.99', '190624111001', '', 1),</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A113" s="6">
         <v>1112</v>
       </c>
@@ -20784,12 +21124,15 @@
         <v>1592</v>
       </c>
       <c r="L113" s="11"/>
-      <c r="M113" s="11" t="str">
+      <c r="M113" s="6">
+        <v>1</v>
+      </c>
+      <c r="N113" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1112, 1112, 2, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 2, 54, '119.99', '190625112001', ''),</v>
-      </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1112, 1112, 2, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 2, 54, '119.99', '190625112001', '', 1),</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A114" s="6">
         <v>1113</v>
       </c>
@@ -20824,12 +21167,15 @@
         <v>1593</v>
       </c>
       <c r="L114" s="11"/>
-      <c r="M114" s="11" t="str">
+      <c r="M114" s="6">
+        <v>1</v>
+      </c>
+      <c r="N114" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1113, 1113, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 2, 59, '109.99', '190625113001', ''),</v>
-      </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1113, 1113, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 2, 59, '109.99', '190625113001', '', 1),</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A115" s="6">
         <v>1114</v>
       </c>
@@ -20864,12 +21210,15 @@
         <v>1594</v>
       </c>
       <c r="L115" s="11"/>
-      <c r="M115" s="11" t="str">
+      <c r="M115" s="6">
+        <v>1</v>
+      </c>
+      <c r="N115" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1114, 1114, 2, DATE_SUB(CURDATE(), INTERVAL 1 DAY), CURDATE(), 1, 0, 1, 74, '119.99', '190625114001', ''),</v>
-      </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1114, 1114, 2, DATE_SUB(CURDATE(), INTERVAL 1 DAY), CURDATE(), 1, 0, 1, 74, '119.99', '190625114001', '', 1),</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A116" s="6">
         <v>1115</v>
       </c>
@@ -20904,12 +21253,15 @@
         <v>1595</v>
       </c>
       <c r="L116" s="11"/>
-      <c r="M116" s="11" t="str">
+      <c r="M116" s="6">
+        <v>1</v>
+      </c>
+      <c r="N116" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1115, 1115, 1, DATE_SUB(CURDATE(), INTERVAL 4 DAY), CURDATE(), 1, 0, 3, 7, '109.99', '190625115001', ''),</v>
-      </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1115, 1115, 1, DATE_SUB(CURDATE(), INTERVAL 4 DAY), CURDATE(), 1, 0, 3, 7, '109.99', '190625115001', '', 1),</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A117" s="6">
         <v>1116</v>
       </c>
@@ -20944,12 +21296,15 @@
         <v>1596</v>
       </c>
       <c r="L117" s="11"/>
-      <c r="M117" s="11" t="str">
+      <c r="M117" s="6">
+        <v>1</v>
+      </c>
+      <c r="N117" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1116, 1116, 3, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 1, 48, '129.99', '190626116001', ''),</v>
-      </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1116, 1116, 3, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 1, 48, '129.99', '190626116001', '', 1),</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A118" s="6">
         <v>1117</v>
       </c>
@@ -20984,12 +21339,15 @@
         <v>1597</v>
       </c>
       <c r="L118" s="11"/>
-      <c r="M118" s="11" t="str">
+      <c r="M118" s="6">
+        <v>1</v>
+      </c>
+      <c r="N118" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1117, 1117, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 2, 61, '109.99', '190626117001', ''),</v>
-      </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1117, 1117, 1, DATE_SUB(CURDATE(), INTERVAL 2 DAY), CURDATE(), 1, 0, 2, 61, '109.99', '190626117001', '', 1),</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A119" s="6">
         <v>1118</v>
       </c>
@@ -21024,12 +21382,15 @@
         <v>1598</v>
       </c>
       <c r="L119" s="11"/>
-      <c r="M119" s="11" t="str">
+      <c r="M119" s="6">
+        <v>1</v>
+      </c>
+      <c r="N119" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1118, 1118, 3, DATE_SUB(CURDATE(), INTERVAL 1 DAY), CURDATE(), 1, 0, 2, 78, '129.99', '190626118001', ''),</v>
-      </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1118, 1118, 3, DATE_SUB(CURDATE(), INTERVAL 1 DAY), CURDATE(), 1, 0, 2, 78, '129.99', '190626118001', '', 1),</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A120" s="6">
         <v>1119</v>
       </c>
@@ -21064,12 +21425,15 @@
         <v>1599</v>
       </c>
       <c r="L120" s="11"/>
-      <c r="M120" s="11" t="str">
+      <c r="M120" s="6">
+        <v>1</v>
+      </c>
+      <c r="N120" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1119, 1119, 1, DATE_SUB(CURDATE(), INTERVAL 1 DAY), CURDATE(), 1, 0, 1, 79, '109.99', '190626119001', ''),</v>
-      </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1119, 1119, 1, DATE_SUB(CURDATE(), INTERVAL 1 DAY), CURDATE(), 1, 0, 1, 79, '109.99', '190626119001', '', 1),</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A121" s="6">
         <v>1120</v>
       </c>
@@ -21104,12 +21468,15 @@
         <v>1600</v>
       </c>
       <c r="L121" s="11"/>
-      <c r="M121" s="11" t="str">
+      <c r="M121" s="6">
+        <v>1</v>
+      </c>
+      <c r="N121" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1120, 1120, 3, DATE_SUB(CURDATE(), INTERVAL 1 DAY), CURDATE(), 1, 0, 3, 80, '129.99', '190627120001', ''),</v>
-      </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1120, 1120, 3, DATE_SUB(CURDATE(), INTERVAL 1 DAY), CURDATE(), 1, 0, 3, 80, '129.99', '190627120001', '', 1),</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A122" s="6">
         <v>1121</v>
       </c>
@@ -21144,12 +21511,15 @@
         <v>1601</v>
       </c>
       <c r="L122" s="11"/>
-      <c r="M122" s="11" t="str">
+      <c r="M122" s="6">
+        <v>1</v>
+      </c>
+      <c r="N122" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1121, 1121, 1, DATE_ADD(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 1, null, '109.99', '190627121001', ''),</v>
-      </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1121, 1121, 1, DATE_ADD(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 1, null, '109.99', '190627121001', '', 1),</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A123" s="6">
         <v>1122</v>
       </c>
@@ -21186,12 +21556,15 @@
       <c r="L123" s="11" t="s">
         <v>1479</v>
       </c>
-      <c r="M123" s="11" t="str">
+      <c r="M123" s="6">
+        <v>1</v>
+      </c>
+      <c r="N123" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1122, 1122, 2, DATE_ADD(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 2, null, '119.99', '190628122001', 'wants a large screen tv'),</v>
-      </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1122, 1122, 2, DATE_ADD(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 2, null, '119.99', '190628122001', 'wants a large screen tv', 1),</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A124" s="6">
         <v>1123</v>
       </c>
@@ -21226,12 +21599,15 @@
         <v>1603</v>
       </c>
       <c r="L124" s="11"/>
-      <c r="M124" s="11" t="str">
+      <c r="M124" s="6">
+        <v>1</v>
+      </c>
+      <c r="N124" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1123, 1123, 1, DATE_ADD(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 0, 0, 2, null, '109.99', '190628123001', ''),</v>
-      </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1123, 1123, 1, DATE_ADD(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 0, 0, 2, null, '109.99', '190628123001', '', 1),</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A125" s="6">
         <v>1124</v>
       </c>
@@ -21266,12 +21642,15 @@
         <v>1604</v>
       </c>
       <c r="L125" s="11"/>
-      <c r="M125" s="11" t="str">
+      <c r="M125" s="6">
+        <v>1</v>
+      </c>
+      <c r="N125" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1124, 1124, 2, DATE_ADD(CURDATE(), INTERVAL 4 DAY), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 1, null, '119.99', '190628124001', ''),</v>
-      </c>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1124, 1124, 2, DATE_ADD(CURDATE(), INTERVAL 4 DAY), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 1, null, '119.99', '190628124001', '', 1),</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A126" s="6">
         <v>1125</v>
       </c>
@@ -21306,12 +21685,15 @@
         <v>1605</v>
       </c>
       <c r="L126" s="11"/>
-      <c r="M126" s="11" t="str">
+      <c r="M126" s="6">
+        <v>1</v>
+      </c>
+      <c r="N126" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1125, 1125, 1, DATE_ADD(CURDATE(), INTERVAL 5 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 3, null, '109.99', '190628125001', ''),</v>
-      </c>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1125, 1125, 1, DATE_ADD(CURDATE(), INTERVAL 5 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 3, null, '109.99', '190628125001', '', 1),</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A127" s="6">
         <v>1126</v>
       </c>
@@ -21346,12 +21728,15 @@
         <v>1606</v>
       </c>
       <c r="L127" s="11"/>
-      <c r="M127" s="11" t="str">
+      <c r="M127" s="6">
+        <v>1</v>
+      </c>
+      <c r="N127" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1126, 1126, 3, DATE_ADD(CURDATE(), INTERVAL 6 DAY), DATE_ADD(CURDATE(), INTERVAL 7 DAY), 0, 0, 1, null, '129.99', '190628126001', ''),</v>
-      </c>
-    </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1126, 1126, 3, DATE_ADD(CURDATE(), INTERVAL 6 DAY), DATE_ADD(CURDATE(), INTERVAL 7 DAY), 0, 0, 1, null, '129.99', '190628126001', '', 1),</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A128" s="6">
         <v>1127</v>
       </c>
@@ -21388,12 +21773,15 @@
       <c r="L128" s="11" t="s">
         <v>1478</v>
       </c>
-      <c r="M128" s="11" t="str">
+      <c r="M128" s="6">
+        <v>1</v>
+      </c>
+      <c r="N128" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1127, 1127, 1, DATE_ADD(CURDATE(), INTERVAL 7 DAY), DATE_ADD(CURDATE(), INTERVAL 8 DAY), 0, 0, 2, null, '109.99', '190629127001', 'needs a late checkout time'),</v>
-      </c>
-    </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1127, 1127, 1, DATE_ADD(CURDATE(), INTERVAL 7 DAY), DATE_ADD(CURDATE(), INTERVAL 8 DAY), 0, 0, 2, null, '109.99', '190629127001', 'needs a late checkout time', 1),</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A129" s="6">
         <v>1128</v>
       </c>
@@ -21428,12 +21816,15 @@
         <v>1608</v>
       </c>
       <c r="L129" s="11"/>
-      <c r="M129" s="11" t="str">
+      <c r="M129" s="6">
+        <v>1</v>
+      </c>
+      <c r="N129" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1128, 1128, 3, DATE_ADD(CURDATE(), INTERVAL 8 DAY), DATE_ADD(CURDATE(), INTERVAL 9 DAY), 0, 0, 2, null, '129.99', '190629128001', ''),</v>
-      </c>
-    </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1128, 1128, 3, DATE_ADD(CURDATE(), INTERVAL 8 DAY), DATE_ADD(CURDATE(), INTERVAL 9 DAY), 0, 0, 2, null, '129.99', '190629128001', '', 1),</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A130" s="6">
         <v>1129</v>
       </c>
@@ -21468,12 +21859,15 @@
         <v>1609</v>
       </c>
       <c r="L130" s="11"/>
-      <c r="M130" s="11" t="str">
+      <c r="M130" s="6">
+        <v>1</v>
+      </c>
+      <c r="N130" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(1129, 1129, 1, DATE_ADD(CURDATE(), INTERVAL 9 DAY), DATE_ADD(CURDATE(), INTERVAL 10 DAY), 0, 0, 1, null, '109.99', '190629129001', ''),</v>
-      </c>
-    </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1129, 1129, 1, DATE_ADD(CURDATE(), INTERVAL 9 DAY), DATE_ADD(CURDATE(), INTERVAL 10 DAY), 0, 0, 1, null, '109.99', '190629129001', '', 1),</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A131" s="6">
         <v>1130</v>
       </c>
@@ -21508,12 +21902,15 @@
         <v>1610</v>
       </c>
       <c r="L131" s="11"/>
-      <c r="M131" s="11" t="str">
-        <f t="shared" ref="M131:M194" si="2">"("&amp;A131&amp;", "&amp;B131&amp;", "&amp;C131&amp;", "&amp;D131&amp;", "&amp;E131&amp;", "&amp;F131&amp;", "&amp;G131&amp;", "&amp;H131&amp;", "&amp;I131&amp;", '"&amp;J131&amp;"', '"&amp;K131&amp;"', '"&amp;L131&amp;"'),"</f>
-        <v>(1130, 1130, 3, DATE_ADD(CURDATE(), INTERVAL 10 DAY), DATE_ADD(CURDATE(), INTERVAL 13 DAY), 0, 0, 3, null, '129.99', '190629130001', ''),</v>
-      </c>
-    </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M131" s="6">
+        <v>1</v>
+      </c>
+      <c r="N131" s="11" t="str">
+        <f t="shared" ref="N131:N194" si="2">"("&amp;A131&amp;", "&amp;B131&amp;", "&amp;C131&amp;", "&amp;D131&amp;", "&amp;E131&amp;", "&amp;F131&amp;", "&amp;G131&amp;", "&amp;H131&amp;", "&amp;I131&amp;", '"&amp;J131&amp;"', '"&amp;K131&amp;"', '"&amp;L131&amp;"', "&amp;M131&amp;"),"</f>
+        <v>(1130, 1130, 3, DATE_ADD(CURDATE(), INTERVAL 10 DAY), DATE_ADD(CURDATE(), INTERVAL 13 DAY), 0, 0, 3, null, '129.99', '190629130001', '', 1),</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A132" s="6">
         <v>1131</v>
       </c>
@@ -21548,12 +21945,15 @@
         <v>1611</v>
       </c>
       <c r="L132" s="11"/>
-      <c r="M132" s="11" t="str">
+      <c r="M132" s="6">
+        <v>1</v>
+      </c>
+      <c r="N132" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1131, 1131, 1, DATE_ADD(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 1, null, '109.99', '190630131001', ''),</v>
-      </c>
-    </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1131, 1131, 1, DATE_ADD(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 1, null, '109.99', '190630131001', '', 1),</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A133" s="6">
         <v>1132</v>
       </c>
@@ -21588,12 +21988,15 @@
         <v>1612</v>
       </c>
       <c r="L133" s="11"/>
-      <c r="M133" s="11" t="str">
+      <c r="M133" s="6">
+        <v>1</v>
+      </c>
+      <c r="N133" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1132, 1132, 2, DATE_ADD(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 2, null, '119.99', '190630132001', ''),</v>
-      </c>
-    </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1132, 1132, 2, DATE_ADD(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 3 DAY), 0, 0, 2, null, '119.99', '190630132001', '', 1),</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A134" s="6">
         <v>1133</v>
       </c>
@@ -21628,12 +22031,15 @@
         <v>1613</v>
       </c>
       <c r="L134" s="11"/>
-      <c r="M134" s="11" t="str">
+      <c r="M134" s="6">
+        <v>1</v>
+      </c>
+      <c r="N134" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1133, 1133, 1, DATE_ADD(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 0, 0, 2, null, '109.99', '190630133001', ''),</v>
-      </c>
-    </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1133, 1133, 1, DATE_ADD(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 0, 0, 2, null, '109.99', '190630133001', '', 1),</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A135" s="6">
         <v>1134</v>
       </c>
@@ -21668,12 +22074,15 @@
         <v>1614</v>
       </c>
       <c r="L135" s="11"/>
-      <c r="M135" s="11" t="str">
+      <c r="M135" s="6">
+        <v>1</v>
+      </c>
+      <c r="N135" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1134, 1134, 2, DATE_ADD(CURDATE(), INTERVAL 4 DAY), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 2, null, '119.99', '190701134001', ''),</v>
-      </c>
-    </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1134, 1134, 2, DATE_ADD(CURDATE(), INTERVAL 4 DAY), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 2, null, '119.99', '190701134001', '', 1),</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A136" s="6">
         <v>1135</v>
       </c>
@@ -21708,12 +22117,15 @@
         <v>1615</v>
       </c>
       <c r="L136" s="11"/>
-      <c r="M136" s="11" t="str">
+      <c r="M136" s="6">
+        <v>1</v>
+      </c>
+      <c r="N136" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1135, 1135, 1, DATE_ADD(CURDATE(), INTERVAL 5 DAY), DATE_ADD(CURDATE(), INTERVAL 8 DAY), 0, 0, 3, null, '109.99', '190701135001', ''),</v>
-      </c>
-    </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1135, 1135, 1, DATE_ADD(CURDATE(), INTERVAL 5 DAY), DATE_ADD(CURDATE(), INTERVAL 8 DAY), 0, 0, 3, null, '109.99', '190701135001', '', 1),</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A137" s="6">
         <v>1136</v>
       </c>
@@ -21748,12 +22160,15 @@
         <v>1616</v>
       </c>
       <c r="L137" s="11"/>
-      <c r="M137" s="11" t="str">
+      <c r="M137" s="6">
+        <v>1</v>
+      </c>
+      <c r="N137" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1136, 1136, 3, DATE_ADD(CURDATE(), INTERVAL 6 DAY), DATE_ADD(CURDATE(), INTERVAL 7 DAY), 0, 0, 4, null, '129.99', '190701136001', ''),</v>
-      </c>
-    </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1136, 1136, 3, DATE_ADD(CURDATE(), INTERVAL 6 DAY), DATE_ADD(CURDATE(), INTERVAL 7 DAY), 0, 0, 4, null, '129.99', '190701136001', '', 1),</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A138" s="6">
         <v>1137</v>
       </c>
@@ -21788,12 +22203,15 @@
         <v>1617</v>
       </c>
       <c r="L138" s="11"/>
-      <c r="M138" s="11" t="str">
+      <c r="M138" s="6">
+        <v>1</v>
+      </c>
+      <c r="N138" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1137, 1137, 1, DATE_ADD(CURDATE(), INTERVAL 7 DAY), DATE_ADD(CURDATE(), INTERVAL 11 DAY), 0, 0, 2, null, '109.99', '190701137001', ''),</v>
-      </c>
-    </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1137, 1137, 1, DATE_ADD(CURDATE(), INTERVAL 7 DAY), DATE_ADD(CURDATE(), INTERVAL 11 DAY), 0, 0, 2, null, '109.99', '190701137001', '', 1),</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A139" s="6">
         <v>1138</v>
       </c>
@@ -21828,12 +22246,15 @@
         <v>1618</v>
       </c>
       <c r="L139" s="11"/>
-      <c r="M139" s="11" t="str">
+      <c r="M139" s="6">
+        <v>1</v>
+      </c>
+      <c r="N139" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1138, 1138, 3, DATE_ADD(CURDATE(), INTERVAL 8 DAY), DATE_ADD(CURDATE(), INTERVAL 9 DAY), 0, 0, 2, null, '129.99', '190701138001', ''),</v>
-      </c>
-    </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1138, 1138, 3, DATE_ADD(CURDATE(), INTERVAL 8 DAY), DATE_ADD(CURDATE(), INTERVAL 9 DAY), 0, 0, 2, null, '129.99', '190701138001', '', 1),</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A140" s="6">
         <v>1139</v>
       </c>
@@ -21868,12 +22289,15 @@
         <v>1619</v>
       </c>
       <c r="L140" s="11"/>
-      <c r="M140" s="11" t="str">
+      <c r="M140" s="6">
+        <v>1</v>
+      </c>
+      <c r="N140" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1139, 1139, 1, DATE_ADD(CURDATE(), INTERVAL 9 DAY), DATE_ADD(CURDATE(), INTERVAL 12 DAY), 0, 0, 1, null, '109.99', '190701139001', ''),</v>
-      </c>
-    </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1139, 1139, 1, DATE_ADD(CURDATE(), INTERVAL 9 DAY), DATE_ADD(CURDATE(), INTERVAL 12 DAY), 0, 0, 1, null, '109.99', '190701139001', '', 1),</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A141" s="6">
         <v>1140</v>
       </c>
@@ -21910,12 +22334,15 @@
       <c r="L141" s="11" t="s">
         <v>1478</v>
       </c>
-      <c r="M141" s="11" t="str">
+      <c r="M141" s="6">
+        <v>1</v>
+      </c>
+      <c r="N141" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1140, 1140, 3, DATE_ADD(CURDATE(), INTERVAL 10 DAY), DATE_ADD(CURDATE(), INTERVAL 13 DAY), 0, 0, 3, null, '129.99', '190701140001', 'needs a late checkout time'),</v>
-      </c>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1140, 1140, 3, DATE_ADD(CURDATE(), INTERVAL 10 DAY), DATE_ADD(CURDATE(), INTERVAL 13 DAY), 0, 0, 3, null, '129.99', '190701140001', 'needs a late checkout time', 1),</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A142" s="6">
         <v>1141</v>
       </c>
@@ -21950,12 +22377,15 @@
         <v>1621</v>
       </c>
       <c r="L142" s="11"/>
-      <c r="M142" s="11" t="str">
+      <c r="M142" s="6">
+        <v>1</v>
+      </c>
+      <c r="N142" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1141, 1141, 1, DATE_ADD(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 1, null, '109.99', '190701141001', ''),</v>
-      </c>
-    </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1141, 1141, 1, DATE_ADD(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 1, null, '109.99', '190701141001', '', 1),</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A143" s="6">
         <v>1142</v>
       </c>
@@ -21990,12 +22420,15 @@
         <v>1622</v>
       </c>
       <c r="L143" s="11"/>
-      <c r="M143" s="11" t="str">
+      <c r="M143" s="6">
+        <v>1</v>
+      </c>
+      <c r="N143" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1142, 1142, 2, DATE_ADD(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 7 DAY), 0, 0, 2, null, '119.99', '190701142001', ''),</v>
-      </c>
-    </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1142, 1142, 2, DATE_ADD(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 7 DAY), 0, 0, 2, null, '119.99', '190701142001', '', 1),</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A144" s="6">
         <v>1143</v>
       </c>
@@ -22030,12 +22463,15 @@
         <v>1623</v>
       </c>
       <c r="L144" s="11"/>
-      <c r="M144" s="11" t="str">
+      <c r="M144" s="6">
+        <v>1</v>
+      </c>
+      <c r="N144" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1143, 1143, 1, DATE_ADD(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 2, null, '109.99', '190702143001', ''),</v>
-      </c>
-    </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1143, 1143, 1, DATE_ADD(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 2, null, '109.99', '190702143001', '', 1),</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A145" s="6">
         <v>1144</v>
       </c>
@@ -22070,12 +22506,15 @@
         <v>1624</v>
       </c>
       <c r="L145" s="11"/>
-      <c r="M145" s="11" t="str">
+      <c r="M145" s="6">
+        <v>1</v>
+      </c>
+      <c r="N145" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1144, 1144, 2, DATE_ADD(CURDATE(), INTERVAL 4 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 1, null, '119.99', '190702144001', ''),</v>
-      </c>
-    </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1144, 1144, 2, DATE_ADD(CURDATE(), INTERVAL 4 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 1, null, '119.99', '190702144001', '', 1),</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A146" s="6">
         <v>1145</v>
       </c>
@@ -22112,12 +22551,15 @@
       <c r="L146" s="11" t="s">
         <v>1480</v>
       </c>
-      <c r="M146" s="11" t="str">
+      <c r="M146" s="6">
+        <v>1</v>
+      </c>
+      <c r="N146" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1145, 1145, 1, DATE_ADD(CURDATE(), INTERVAL 5 DAY), DATE_ADD(CURDATE(), INTERVAL 12 DAY), 0, 0, 3, null, '109.99', '190702145001', 'wants a good view'),</v>
-      </c>
-    </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1145, 1145, 1, DATE_ADD(CURDATE(), INTERVAL 5 DAY), DATE_ADD(CURDATE(), INTERVAL 12 DAY), 0, 0, 3, null, '109.99', '190702145001', 'wants a good view', 1),</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A147" s="6">
         <v>1146</v>
       </c>
@@ -22152,12 +22594,15 @@
         <v>1626</v>
       </c>
       <c r="L147" s="11"/>
-      <c r="M147" s="11" t="str">
+      <c r="M147" s="6">
+        <v>1</v>
+      </c>
+      <c r="N147" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1146, 1146, 3, DATE_ADD(CURDATE(), INTERVAL 6 DAY), DATE_ADD(CURDATE(), INTERVAL 12 DAY), 0, 0, 4, null, '129.99', '190702146001', ''),</v>
-      </c>
-    </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1146, 1146, 3, DATE_ADD(CURDATE(), INTERVAL 6 DAY), DATE_ADD(CURDATE(), INTERVAL 12 DAY), 0, 0, 4, null, '129.99', '190702146001', '', 1),</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A148" s="6">
         <v>1147</v>
       </c>
@@ -22192,12 +22637,15 @@
         <v>1627</v>
       </c>
       <c r="L148" s="11"/>
-      <c r="M148" s="11" t="str">
+      <c r="M148" s="6">
+        <v>1</v>
+      </c>
+      <c r="N148" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1147, 1147, 1, DATE_ADD(CURDATE(), INTERVAL 7 DAY), DATE_ADD(CURDATE(), INTERVAL 12 DAY), 0, 0, 2, null, '109.99', '190702147001', ''),</v>
-      </c>
-    </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1147, 1147, 1, DATE_ADD(CURDATE(), INTERVAL 7 DAY), DATE_ADD(CURDATE(), INTERVAL 12 DAY), 0, 0, 2, null, '109.99', '190702147001', '', 1),</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A149" s="6">
         <v>1148</v>
       </c>
@@ -22234,12 +22682,15 @@
       <c r="L149" s="11" t="s">
         <v>1478</v>
       </c>
-      <c r="M149" s="11" t="str">
+      <c r="M149" s="6">
+        <v>1</v>
+      </c>
+      <c r="N149" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1148, 1148, 3, DATE_ADD(CURDATE(), INTERVAL 8 DAY), DATE_ADD(CURDATE(), INTERVAL 11 DAY), 0, 0, 2, null, '129.99', '190703148001', 'needs a late checkout time'),</v>
-      </c>
-    </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1148, 1148, 3, DATE_ADD(CURDATE(), INTERVAL 8 DAY), DATE_ADD(CURDATE(), INTERVAL 11 DAY), 0, 0, 2, null, '129.99', '190703148001', 'needs a late checkout time', 1),</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A150" s="6">
         <v>1149</v>
       </c>
@@ -22274,12 +22725,15 @@
         <v>1629</v>
       </c>
       <c r="L150" s="11"/>
-      <c r="M150" s="11" t="str">
+      <c r="M150" s="6">
+        <v>1</v>
+      </c>
+      <c r="N150" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1149, 1149, 1, DATE_ADD(CURDATE(), INTERVAL 9 DAY), DATE_ADD(CURDATE(), INTERVAL 10 DAY), 0, 0, 1, null, '109.99', '190703149001', ''),</v>
-      </c>
-    </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1149, 1149, 1, DATE_ADD(CURDATE(), INTERVAL 9 DAY), DATE_ADD(CURDATE(), INTERVAL 10 DAY), 0, 0, 1, null, '109.99', '190703149001', '', 1),</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A151" s="6">
         <v>1150</v>
       </c>
@@ -22314,12 +22768,15 @@
         <v>1630</v>
       </c>
       <c r="L151" s="11"/>
-      <c r="M151" s="11" t="str">
+      <c r="M151" s="6">
+        <v>1</v>
+      </c>
+      <c r="N151" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1150, 1150, 3, DATE_ADD(CURDATE(), INTERVAL 10 DAY), DATE_ADD(CURDATE(), INTERVAL 12 DAY), 0, 0, 3, null, '129.99', '190703150001', ''),</v>
-      </c>
-    </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1150, 1150, 3, DATE_ADD(CURDATE(), INTERVAL 10 DAY), DATE_ADD(CURDATE(), INTERVAL 12 DAY), 0, 0, 3, null, '129.99', '190703150001', '', 1),</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A152" s="6">
         <v>1151</v>
       </c>
@@ -22354,12 +22811,15 @@
         <v>1631</v>
       </c>
       <c r="L152" s="11"/>
-      <c r="M152" s="11" t="str">
+      <c r="M152" s="6">
+        <v>1</v>
+      </c>
+      <c r="N152" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1151, 1151, 1, DATE_ADD(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 7 DAY), 0, 0, 1, null, '109.99', '190703151001', ''),</v>
-      </c>
-    </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1151, 1151, 1, DATE_ADD(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 7 DAY), 0, 0, 1, null, '109.99', '190703151001', '', 1),</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A153" s="6">
         <v>1152</v>
       </c>
@@ -22394,12 +22854,15 @@
         <v>1632</v>
       </c>
       <c r="L153" s="11"/>
-      <c r="M153" s="11" t="str">
+      <c r="M153" s="6">
+        <v>1</v>
+      </c>
+      <c r="N153" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1152, 1152, 2, DATE_ADD(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 2, null, '119.99', '190703152001', ''),</v>
-      </c>
-    </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1152, 1152, 2, DATE_ADD(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 2, null, '119.99', '190703152001', '', 1),</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A154" s="6">
         <v>1153</v>
       </c>
@@ -22434,12 +22897,15 @@
         <v>1633</v>
       </c>
       <c r="L154" s="11"/>
-      <c r="M154" s="11" t="str">
+      <c r="M154" s="6">
+        <v>1</v>
+      </c>
+      <c r="N154" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1153, 1153, 1, DATE_ADD(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 2, null, '109.99', '190703153001', ''),</v>
-      </c>
-    </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1153, 1153, 1, DATE_ADD(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 2, null, '109.99', '190703153001', '', 1),</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A155" s="6">
         <v>1154</v>
       </c>
@@ -22474,12 +22940,15 @@
         <v>1634</v>
       </c>
       <c r="L155" s="11"/>
-      <c r="M155" s="11" t="str">
+      <c r="M155" s="6">
+        <v>1</v>
+      </c>
+      <c r="N155" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1154, 1154, 2, DATE_ADD(CURDATE(), INTERVAL 4 DAY), DATE_ADD(CURDATE(), INTERVAL 12 DAY), 0, 0, 1, null, '119.99', '190703154001', ''),</v>
-      </c>
-    </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1154, 1154, 2, DATE_ADD(CURDATE(), INTERVAL 4 DAY), DATE_ADD(CURDATE(), INTERVAL 12 DAY), 0, 0, 1, null, '119.99', '190703154001', '', 1),</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A156" s="6">
         <v>1155</v>
       </c>
@@ -22514,12 +22983,15 @@
         <v>1635</v>
       </c>
       <c r="L156" s="11"/>
-      <c r="M156" s="11" t="str">
+      <c r="M156" s="6">
+        <v>1</v>
+      </c>
+      <c r="N156" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1155, 1155, 1, DATE_ADD(CURDATE(), INTERVAL 5 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 3, null, '109.99', '190703155001', ''),</v>
-      </c>
-    </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1155, 1155, 1, DATE_ADD(CURDATE(), INTERVAL 5 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 3, null, '109.99', '190703155001', '', 1),</v>
+      </c>
+    </row>
+    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A157" s="6">
         <v>1156</v>
       </c>
@@ -22554,12 +23026,15 @@
         <v>1636</v>
       </c>
       <c r="L157" s="11"/>
-      <c r="M157" s="11" t="str">
+      <c r="M157" s="6">
+        <v>1</v>
+      </c>
+      <c r="N157" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1156, 1156, 3, DATE_ADD(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 4, null, '129.99', '190703156001', ''),</v>
-      </c>
-    </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1156, 1156, 3, DATE_ADD(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 4, null, '129.99', '190703156001', '', 1),</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A158" s="6">
         <v>1157</v>
       </c>
@@ -22594,12 +23069,15 @@
         <v>1637</v>
       </c>
       <c r="L158" s="11"/>
-      <c r="M158" s="11" t="str">
+      <c r="M158" s="6">
+        <v>1</v>
+      </c>
+      <c r="N158" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1157, 1157, 1, DATE_ADD(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 2, null, '109.99', '190703157001', ''),</v>
-      </c>
-    </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1157, 1157, 1, DATE_ADD(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 2, null, '109.99', '190703157001', '', 1),</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A159" s="6">
         <v>1158</v>
       </c>
@@ -22634,12 +23112,15 @@
         <v>1638</v>
       </c>
       <c r="L159" s="11"/>
-      <c r="M159" s="11" t="str">
+      <c r="M159" s="6">
+        <v>1</v>
+      </c>
+      <c r="N159" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1158, 1158, 3, DATE_ADD(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 7 DAY), 0, 0, 2, null, '129.99', '190703158001', ''),</v>
-      </c>
-    </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1158, 1158, 3, DATE_ADD(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 7 DAY), 0, 0, 2, null, '129.99', '190703158001', '', 1),</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A160" s="6">
         <v>1159</v>
       </c>
@@ -22676,12 +23157,15 @@
       <c r="L160" s="11" t="s">
         <v>1478</v>
       </c>
-      <c r="M160" s="11" t="str">
+      <c r="M160" s="6">
+        <v>1</v>
+      </c>
+      <c r="N160" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1159, 1159, 1, DATE_ADD(CURDATE(), INTERVAL 4 DAY), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 1, null, '109.99', '190703159001', 'needs a late checkout time'),</v>
-      </c>
-    </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1159, 1159, 1, DATE_ADD(CURDATE(), INTERVAL 4 DAY), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 1, null, '109.99', '190703159001', 'needs a late checkout time', 1),</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A161" s="6">
         <v>1160</v>
       </c>
@@ -22716,12 +23200,15 @@
         <v>1640</v>
       </c>
       <c r="L161" s="11"/>
-      <c r="M161" s="11" t="str">
+      <c r="M161" s="6">
+        <v>1</v>
+      </c>
+      <c r="N161" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1160, 1160, 3, DATE_ADD(CURDATE(), INTERVAL 5 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 3, null, '129.99', '190703160001', ''),</v>
-      </c>
-    </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1160, 1160, 3, DATE_ADD(CURDATE(), INTERVAL 5 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 3, null, '129.99', '190703160001', '', 1),</v>
+      </c>
+    </row>
+    <row r="162" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A162" s="6">
         <v>1161</v>
       </c>
@@ -22756,12 +23243,15 @@
         <v>1641</v>
       </c>
       <c r="L162" s="11"/>
-      <c r="M162" s="11" t="str">
+      <c r="M162" s="6">
+        <v>1</v>
+      </c>
+      <c r="N162" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1161, 1161, 1, DATE_ADD(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 12 DAY), 0, 0, 1, null, '109.99', '190703161001', ''),</v>
-      </c>
-    </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1161, 1161, 1, DATE_ADD(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 12 DAY), 0, 0, 1, null, '109.99', '190703161001', '', 1),</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A163" s="6">
         <v>1162</v>
       </c>
@@ -22796,12 +23286,15 @@
         <v>1642</v>
       </c>
       <c r="L163" s="11"/>
-      <c r="M163" s="11" t="str">
+      <c r="M163" s="6">
+        <v>1</v>
+      </c>
+      <c r="N163" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1162, 1162, 2, DATE_ADD(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 2, null, '119.99', '190703162001', ''),</v>
-      </c>
-    </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1162, 1162, 2, DATE_ADD(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 2, null, '119.99', '190703162001', '', 1),</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A164" s="6">
         <v>1163</v>
       </c>
@@ -22836,12 +23329,15 @@
         <v>1643</v>
       </c>
       <c r="L164" s="11"/>
-      <c r="M164" s="11" t="str">
+      <c r="M164" s="6">
+        <v>1</v>
+      </c>
+      <c r="N164" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1163, 1163, 1, DATE_ADD(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 2, null, '109.99', '190703163001', ''),</v>
-      </c>
-    </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1163, 1163, 1, DATE_ADD(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 2, null, '109.99', '190703163001', '', 1),</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A165" s="6">
         <v>1164</v>
       </c>
@@ -22876,12 +23372,15 @@
         <v>1644</v>
       </c>
       <c r="L165" s="11"/>
-      <c r="M165" s="11" t="str">
+      <c r="M165" s="6">
+        <v>1</v>
+      </c>
+      <c r="N165" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1164, 1164, 2, DATE_ADD(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 2, null, '119.99', '190703164001', ''),</v>
-      </c>
-    </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1164, 1164, 2, DATE_ADD(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 2 DAY), 0, 0, 2, null, '119.99', '190703164001', '', 1),</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A166" s="6">
         <v>1165</v>
       </c>
@@ -22916,12 +23415,15 @@
         <v>1645</v>
       </c>
       <c r="L166" s="11"/>
-      <c r="M166" s="11" t="str">
+      <c r="M166" s="6">
+        <v>1</v>
+      </c>
+      <c r="N166" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1165, 1165, 1, DATE_ADD(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 3, null, '109.99', '190703165001', ''),</v>
-      </c>
-    </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1165, 1165, 1, DATE_ADD(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 3, null, '109.99', '190703165001', '', 1),</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A167" s="6">
         <v>1166</v>
       </c>
@@ -22956,12 +23458,15 @@
         <v>1646</v>
       </c>
       <c r="L167" s="11"/>
-      <c r="M167" s="11" t="str">
+      <c r="M167" s="6">
+        <v>1</v>
+      </c>
+      <c r="N167" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1166, 1166, 3, DATE_ADD(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 0, 0, 2, null, '129.99', '190703166001', ''),</v>
-      </c>
-    </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1166, 1166, 3, DATE_ADD(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 4 DAY), 0, 0, 2, null, '129.99', '190703166001', '', 1),</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A168" s="6">
         <v>1167</v>
       </c>
@@ -22998,12 +23503,15 @@
       <c r="L168" s="11" t="s">
         <v>1479</v>
       </c>
-      <c r="M168" s="11" t="str">
+      <c r="M168" s="6">
+        <v>1</v>
+      </c>
+      <c r="N168" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1167, 1167, 1, DATE_ADD(CURDATE(), INTERVAL 12 DAY), DATE_ADD(CURDATE(), INTERVAL 15 DAY), 0, 0, 2, null, '109.99', '190704167001', 'wants a large screen tv'),</v>
-      </c>
-    </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1167, 1167, 1, DATE_ADD(CURDATE(), INTERVAL 12 DAY), DATE_ADD(CURDATE(), INTERVAL 15 DAY), 0, 0, 2, null, '109.99', '190704167001', 'wants a large screen tv', 1),</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A169" s="6">
         <v>1168</v>
       </c>
@@ -23038,12 +23546,15 @@
         <v>1648</v>
       </c>
       <c r="L169" s="11"/>
-      <c r="M169" s="11" t="str">
+      <c r="M169" s="6">
+        <v>1</v>
+      </c>
+      <c r="N169" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1168, 1168, 3, DATE_ADD(CURDATE(), INTERVAL 12 DAY), DATE_ADD(CURDATE(), INTERVAL 15 DAY), 0, 0, 2, null, '129.99', '190704168001', ''),</v>
-      </c>
-    </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1168, 1168, 3, DATE_ADD(CURDATE(), INTERVAL 12 DAY), DATE_ADD(CURDATE(), INTERVAL 15 DAY), 0, 0, 2, null, '129.99', '190704168001', '', 1),</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A170" s="6">
         <v>1169</v>
       </c>
@@ -23078,12 +23589,15 @@
         <v>1649</v>
       </c>
       <c r="L170" s="11"/>
-      <c r="M170" s="11" t="str">
+      <c r="M170" s="6">
+        <v>1</v>
+      </c>
+      <c r="N170" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1169, 1169, 1, DATE_ADD(CURDATE(), INTERVAL 13 DAY), DATE_ADD(CURDATE(), INTERVAL 15 DAY), 0, 0, 1, null, '109.99', '190704169001', ''),</v>
-      </c>
-    </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1169, 1169, 1, DATE_ADD(CURDATE(), INTERVAL 13 DAY), DATE_ADD(CURDATE(), INTERVAL 15 DAY), 0, 0, 1, null, '109.99', '190704169001', '', 1),</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A171" s="6">
         <v>1170</v>
       </c>
@@ -23118,12 +23632,15 @@
         <v>1650</v>
       </c>
       <c r="L171" s="11"/>
-      <c r="M171" s="11" t="str">
+      <c r="M171" s="6">
+        <v>1</v>
+      </c>
+      <c r="N171" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1170, 1170, 3, DATE_ADD(CURDATE(), INTERVAL 14 DAY), DATE_ADD(CURDATE(), INTERVAL 15 DAY), 0, 0, 3, null, '129.99', '190704170001', ''),</v>
-      </c>
-    </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1170, 1170, 3, DATE_ADD(CURDATE(), INTERVAL 14 DAY), DATE_ADD(CURDATE(), INTERVAL 15 DAY), 0, 0, 3, null, '129.99', '190704170001', '', 1),</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A172" s="6">
         <v>1171</v>
       </c>
@@ -23158,12 +23675,15 @@
         <v>1651</v>
       </c>
       <c r="L172" s="11"/>
-      <c r="M172" s="11" t="str">
+      <c r="M172" s="6">
+        <v>1</v>
+      </c>
+      <c r="N172" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1171, 1171, 1, DATE_ADD(CURDATE(), INTERVAL 16 DAY), DATE_ADD(CURDATE(), INTERVAL 19 DAY), 0, 0, 1, null, '109.99', '190704171001', ''),</v>
-      </c>
-    </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1171, 1171, 1, DATE_ADD(CURDATE(), INTERVAL 16 DAY), DATE_ADD(CURDATE(), INTERVAL 19 DAY), 0, 0, 1, null, '109.99', '190704171001', '', 1),</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A173" s="6">
         <v>1172</v>
       </c>
@@ -23198,12 +23718,15 @@
         <v>1652</v>
       </c>
       <c r="L173" s="11"/>
-      <c r="M173" s="11" t="str">
+      <c r="M173" s="6">
+        <v>1</v>
+      </c>
+      <c r="N173" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1172, 1172, 2, DATE_ADD(CURDATE(), INTERVAL 22 DAY), DATE_ADD(CURDATE(), INTERVAL 23 DAY), 0, 0, 2, null, '119.99', '190704172001', ''),</v>
-      </c>
-    </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1172, 1172, 2, DATE_ADD(CURDATE(), INTERVAL 22 DAY), DATE_ADD(CURDATE(), INTERVAL 23 DAY), 0, 0, 2, null, '119.99', '190704172001', '', 1),</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A174" s="6">
         <v>1173</v>
       </c>
@@ -23238,12 +23761,15 @@
         <v>1653</v>
       </c>
       <c r="L174" s="11"/>
-      <c r="M174" s="11" t="str">
+      <c r="M174" s="6">
+        <v>1</v>
+      </c>
+      <c r="N174" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1173, 1173, 1, DATE_ADD(CURDATE(), INTERVAL 28 DAY), DATE_ADD(CURDATE(), INTERVAL 29 DAY), 0, 0, 2, null, '109.99', '190704173001', ''),</v>
-      </c>
-    </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1173, 1173, 1, DATE_ADD(CURDATE(), INTERVAL 28 DAY), DATE_ADD(CURDATE(), INTERVAL 29 DAY), 0, 0, 2, null, '109.99', '190704173001', '', 1),</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A175" s="6">
         <v>1174</v>
       </c>
@@ -23278,12 +23804,15 @@
         <v>1654</v>
       </c>
       <c r="L175" s="11"/>
-      <c r="M175" s="11" t="str">
+      <c r="M175" s="6">
+        <v>1</v>
+      </c>
+      <c r="N175" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1174, 1174, 2, DATE_ADD(CURDATE(), INTERVAL 30 DAY), DATE_ADD(CURDATE(), INTERVAL 36 DAY), 0, 0, 1, null, '119.99', '190704174001', ''),</v>
-      </c>
-    </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1174, 1174, 2, DATE_ADD(CURDATE(), INTERVAL 30 DAY), DATE_ADD(CURDATE(), INTERVAL 36 DAY), 0, 0, 1, null, '119.99', '190704174001', '', 1),</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A176" s="6">
         <v>1175</v>
       </c>
@@ -23318,12 +23847,15 @@
         <v>1655</v>
       </c>
       <c r="L176" s="11"/>
-      <c r="M176" s="11" t="str">
+      <c r="M176" s="6">
+        <v>1</v>
+      </c>
+      <c r="N176" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1175, 1175, 1, DATE_ADD(CURDATE(), INTERVAL 35 DAY), DATE_ADD(CURDATE(), INTERVAL 38 DAY), 0, 0, 3, null, '109.99', '190705175001', ''),</v>
-      </c>
-    </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1175, 1175, 1, DATE_ADD(CURDATE(), INTERVAL 35 DAY), DATE_ADD(CURDATE(), INTERVAL 38 DAY), 0, 0, 3, null, '109.99', '190705175001', '', 1),</v>
+      </c>
+    </row>
+    <row r="177" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A177" s="6">
         <v>1176</v>
       </c>
@@ -23358,12 +23890,15 @@
         <v>1656</v>
       </c>
       <c r="L177" s="11"/>
-      <c r="M177" s="11" t="str">
+      <c r="M177" s="6">
+        <v>1</v>
+      </c>
+      <c r="N177" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1176, 1176, 3, DATE_ADD(CURDATE(), INTERVAL 42 DAY), DATE_ADD(CURDATE(), INTERVAL 44 DAY), 0, 0, 1, null, '129.99', '190705176001', ''),</v>
-      </c>
-    </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1176, 1176, 3, DATE_ADD(CURDATE(), INTERVAL 42 DAY), DATE_ADD(CURDATE(), INTERVAL 44 DAY), 0, 0, 1, null, '129.99', '190705176001', '', 1),</v>
+      </c>
+    </row>
+    <row r="178" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A178" s="6">
         <v>1177</v>
       </c>
@@ -23400,12 +23935,15 @@
       <c r="L178" s="11" t="s">
         <v>1478</v>
       </c>
-      <c r="M178" s="11" t="str">
+      <c r="M178" s="6">
+        <v>1</v>
+      </c>
+      <c r="N178" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1177, 1177, 1, DATE_ADD(CURDATE(), INTERVAL 45 DAY), DATE_ADD(CURDATE(), INTERVAL 48 DAY), 0, 0, 2, null, '109.99', '190705177001', 'needs a late checkout time'),</v>
-      </c>
-    </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1177, 1177, 1, DATE_ADD(CURDATE(), INTERVAL 45 DAY), DATE_ADD(CURDATE(), INTERVAL 48 DAY), 0, 0, 2, null, '109.99', '190705177001', 'needs a late checkout time', 1),</v>
+      </c>
+    </row>
+    <row r="179" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A179" s="6">
         <v>1178</v>
       </c>
@@ -23440,12 +23978,15 @@
         <v>1658</v>
       </c>
       <c r="L179" s="11"/>
-      <c r="M179" s="11" t="str">
+      <c r="M179" s="6">
+        <v>1</v>
+      </c>
+      <c r="N179" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1178, 1178, 3, DATE_ADD(CURDATE(), INTERVAL 47 DAY), DATE_ADD(CURDATE(), INTERVAL 49 DAY), 0, 0, 2, null, '129.99', '190705178001', ''),</v>
-      </c>
-    </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1178, 1178, 3, DATE_ADD(CURDATE(), INTERVAL 47 DAY), DATE_ADD(CURDATE(), INTERVAL 49 DAY), 0, 0, 2, null, '129.99', '190705178001', '', 1),</v>
+      </c>
+    </row>
+    <row r="180" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A180" s="6">
         <v>1179</v>
       </c>
@@ -23480,12 +24021,15 @@
         <v>1659</v>
       </c>
       <c r="L180" s="11"/>
-      <c r="M180" s="11" t="str">
+      <c r="M180" s="6">
+        <v>1</v>
+      </c>
+      <c r="N180" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1179, 1179, 1, DATE_ADD(CURDATE(), INTERVAL 49 DAY), DATE_ADD(CURDATE(), INTERVAL 52 DAY), 0, 0, 1, null, '109.99', '190705179001', ''),</v>
-      </c>
-    </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1179, 1179, 1, DATE_ADD(CURDATE(), INTERVAL 49 DAY), DATE_ADD(CURDATE(), INTERVAL 52 DAY), 0, 0, 1, null, '109.99', '190705179001', '', 1),</v>
+      </c>
+    </row>
+    <row r="181" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A181" s="6">
         <v>1180</v>
       </c>
@@ -23520,12 +24064,15 @@
         <v>1660</v>
       </c>
       <c r="L181" s="11"/>
-      <c r="M181" s="11" t="str">
+      <c r="M181" s="6">
+        <v>1</v>
+      </c>
+      <c r="N181" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1180, 1180, 3, DATE_ADD(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 3, null, '129.99', '190706180001', ''),</v>
-      </c>
-    </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1180, 1180, 3, DATE_ADD(CURDATE(), INTERVAL 1 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 3, null, '129.99', '190706180001', '', 1),</v>
+      </c>
+    </row>
+    <row r="182" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A182" s="6">
         <v>1181</v>
       </c>
@@ -23560,12 +24107,15 @@
         <v>1661</v>
       </c>
       <c r="L182" s="11"/>
-      <c r="M182" s="11" t="str">
+      <c r="M182" s="6">
+        <v>1</v>
+      </c>
+      <c r="N182" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1181, 1181, 1, DATE_ADD(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 7 DAY), 0, 0, 1, null, '109.99', '190706181001', ''),</v>
-      </c>
-    </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1181, 1181, 1, DATE_ADD(CURDATE(), INTERVAL 2 DAY), DATE_ADD(CURDATE(), INTERVAL 7 DAY), 0, 0, 1, null, '109.99', '190706181001', '', 1),</v>
+      </c>
+    </row>
+    <row r="183" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A183" s="6">
         <v>1182</v>
       </c>
@@ -23600,12 +24150,15 @@
         <v>1662</v>
       </c>
       <c r="L183" s="11"/>
-      <c r="M183" s="11" t="str">
+      <c r="M183" s="6">
+        <v>1</v>
+      </c>
+      <c r="N183" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1182, 1182, 2, DATE_ADD(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 2, null, '119.99', '190706182001', ''),</v>
-      </c>
-    </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1182, 1182, 2, DATE_ADD(CURDATE(), INTERVAL 3 DAY), DATE_ADD(CURDATE(), INTERVAL 5 DAY), 0, 0, 2, null, '119.99', '190706182001', '', 1),</v>
+      </c>
+    </row>
+    <row r="184" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A184" s="6">
         <v>1183</v>
       </c>
@@ -23640,12 +24193,15 @@
         <v>1663</v>
       </c>
       <c r="L184" s="11"/>
-      <c r="M184" s="11" t="str">
+      <c r="M184" s="6">
+        <v>1</v>
+      </c>
+      <c r="N184" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1183, 1183, 1, DATE_ADD(CURDATE(), INTERVAL 4 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 2, null, '109.99', '190707183001', ''),</v>
-      </c>
-    </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1183, 1183, 1, DATE_ADD(CURDATE(), INTERVAL 4 DAY), DATE_ADD(CURDATE(), INTERVAL 6 DAY), 0, 0, 2, null, '109.99', '190707183001', '', 1),</v>
+      </c>
+    </row>
+    <row r="185" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A185" s="6">
         <v>1184</v>
       </c>
@@ -23680,12 +24236,15 @@
         <v>1664</v>
       </c>
       <c r="L185" s="11"/>
-      <c r="M185" s="11" t="str">
+      <c r="M185" s="6">
+        <v>1</v>
+      </c>
+      <c r="N185" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1184, 1184, 2, DATE_ADD(CURDATE(), INTERVAL 5 DAY), DATE_ADD(CURDATE(), INTERVAL 9 DAY), 0, 0, 1, null, '119.99', '190707184001', ''),</v>
-      </c>
-    </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1184, 1184, 2, DATE_ADD(CURDATE(), INTERVAL 5 DAY), DATE_ADD(CURDATE(), INTERVAL 9 DAY), 0, 0, 1, null, '119.99', '190707184001', '', 1),</v>
+      </c>
+    </row>
+    <row r="186" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A186" s="6">
         <v>1185</v>
       </c>
@@ -23720,12 +24279,15 @@
         <v>1665</v>
       </c>
       <c r="L186" s="11"/>
-      <c r="M186" s="11" t="str">
+      <c r="M186" s="6">
+        <v>1</v>
+      </c>
+      <c r="N186" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1185, 1185, 1, DATE_ADD(CURDATE(), INTERVAL 6 DAY), DATE_ADD(CURDATE(), INTERVAL 9 DAY), 0, 0, 3, null, '109.99', '190707185001', ''),</v>
-      </c>
-    </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1185, 1185, 1, DATE_ADD(CURDATE(), INTERVAL 6 DAY), DATE_ADD(CURDATE(), INTERVAL 9 DAY), 0, 0, 3, null, '109.99', '190707185001', '', 1),</v>
+      </c>
+    </row>
+    <row r="187" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A187" s="6">
         <v>1186</v>
       </c>
@@ -23760,12 +24322,15 @@
         <v>1666</v>
       </c>
       <c r="L187" s="11"/>
-      <c r="M187" s="11" t="str">
+      <c r="M187" s="6">
+        <v>1</v>
+      </c>
+      <c r="N187" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1186, 1186, 3, DATE_ADD(CURDATE(), INTERVAL 7 DAY), DATE_ADD(CURDATE(), INTERVAL 8 DAY), 0, 0, 1, null, '129.99', '190708186001', ''),</v>
-      </c>
-    </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1186, 1186, 3, DATE_ADD(CURDATE(), INTERVAL 7 DAY), DATE_ADD(CURDATE(), INTERVAL 8 DAY), 0, 0, 1, null, '129.99', '190708186001', '', 1),</v>
+      </c>
+    </row>
+    <row r="188" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A188" s="6">
         <v>1187</v>
       </c>
@@ -23802,12 +24367,15 @@
       <c r="L188" s="11" t="s">
         <v>1478</v>
       </c>
-      <c r="M188" s="11" t="str">
+      <c r="M188" s="6">
+        <v>1</v>
+      </c>
+      <c r="N188" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1187, 1187, 1, DATE_ADD(CURDATE(), INTERVAL 8 DAY), DATE_ADD(CURDATE(), INTERVAL 11 DAY), 0, 0, 2, null, '109.99', '190708187001', 'needs a late checkout time'),</v>
-      </c>
-    </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1187, 1187, 1, DATE_ADD(CURDATE(), INTERVAL 8 DAY), DATE_ADD(CURDATE(), INTERVAL 11 DAY), 0, 0, 2, null, '109.99', '190708187001', 'needs a late checkout time', 1),</v>
+      </c>
+    </row>
+    <row r="189" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A189" s="6">
         <v>1188</v>
       </c>
@@ -23842,12 +24410,15 @@
         <v>1668</v>
       </c>
       <c r="L189" s="11"/>
-      <c r="M189" s="11" t="str">
+      <c r="M189" s="6">
+        <v>1</v>
+      </c>
+      <c r="N189" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1188, 1188, 3, DATE_ADD(CURDATE(), INTERVAL 9 DAY), DATE_ADD(CURDATE(), INTERVAL 10 DAY), 0, 0, 2, null, '129.99', '190709188001', ''),</v>
-      </c>
-    </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1188, 1188, 3, DATE_ADD(CURDATE(), INTERVAL 9 DAY), DATE_ADD(CURDATE(), INTERVAL 10 DAY), 0, 0, 2, null, '129.99', '190709188001', '', 1),</v>
+      </c>
+    </row>
+    <row r="190" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A190" s="6">
         <v>1189</v>
       </c>
@@ -23882,12 +24453,15 @@
         <v>1669</v>
       </c>
       <c r="L190" s="11"/>
-      <c r="M190" s="11" t="str">
+      <c r="M190" s="6">
+        <v>1</v>
+      </c>
+      <c r="N190" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1189, 1189, 1, DATE_ADD(CURDATE(), INTERVAL 10 DAY), DATE_ADD(CURDATE(), INTERVAL 12 DAY), 0, 0, 1, null, '109.99', '190709189001', ''),</v>
-      </c>
-    </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1189, 1189, 1, DATE_ADD(CURDATE(), INTERVAL 10 DAY), DATE_ADD(CURDATE(), INTERVAL 12 DAY), 0, 0, 1, null, '109.99', '190709189001', '', 1),</v>
+      </c>
+    </row>
+    <row r="191" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A191" s="6">
         <v>1190</v>
       </c>
@@ -23922,12 +24496,15 @@
         <v>1670</v>
       </c>
       <c r="L191" s="11"/>
-      <c r="M191" s="11" t="str">
+      <c r="M191" s="6">
+        <v>1</v>
+      </c>
+      <c r="N191" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1190, 1190, 3, DATE_ADD(CURDATE(), INTERVAL 68 DAY), DATE_ADD(CURDATE(), INTERVAL 71 DAY), 0, 0, 3, null, '129.99', '190710190001', ''),</v>
-      </c>
-    </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1190, 1190, 3, DATE_ADD(CURDATE(), INTERVAL 68 DAY), DATE_ADD(CURDATE(), INTERVAL 71 DAY), 0, 0, 3, null, '129.99', '190710190001', '', 1),</v>
+      </c>
+    </row>
+    <row r="192" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A192" s="6">
         <v>1191</v>
       </c>
@@ -23964,12 +24541,15 @@
       <c r="L192" s="11" t="s">
         <v>1480</v>
       </c>
-      <c r="M192" s="11" t="str">
+      <c r="M192" s="6">
+        <v>1</v>
+      </c>
+      <c r="N192" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1191, 1191, 1, DATE_ADD(CURDATE(), INTERVAL 75 DAY), DATE_ADD(CURDATE(), INTERVAL 77 DAY), 0, 0, 1, null, '109.99', '190710191001', 'wants a good view'),</v>
-      </c>
-    </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1191, 1191, 1, DATE_ADD(CURDATE(), INTERVAL 75 DAY), DATE_ADD(CURDATE(), INTERVAL 77 DAY), 0, 0, 1, null, '109.99', '190710191001', 'wants a good view', 1),</v>
+      </c>
+    </row>
+    <row r="193" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A193" s="6">
         <v>1192</v>
       </c>
@@ -24004,12 +24584,15 @@
         <v>1672</v>
       </c>
       <c r="L193" s="11"/>
-      <c r="M193" s="11" t="str">
+      <c r="M193" s="6">
+        <v>1</v>
+      </c>
+      <c r="N193" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1192, 1192, 2, DATE_ADD(CURDATE(), INTERVAL 81 DAY), DATE_ADD(CURDATE(), INTERVAL 84 DAY), 0, 0, 2, null, '119.99', '190711192001', ''),</v>
-      </c>
-    </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1192, 1192, 2, DATE_ADD(CURDATE(), INTERVAL 81 DAY), DATE_ADD(CURDATE(), INTERVAL 84 DAY), 0, 0, 2, null, '119.99', '190711192001', '', 1),</v>
+      </c>
+    </row>
+    <row r="194" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A194" s="6">
         <v>1193</v>
       </c>
@@ -24044,12 +24627,15 @@
         <v>1673</v>
       </c>
       <c r="L194" s="11"/>
-      <c r="M194" s="11" t="str">
+      <c r="M194" s="6">
+        <v>1</v>
+      </c>
+      <c r="N194" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>(1193, 1193, 1, DATE_ADD(CURDATE(), INTERVAL 85 DAY), DATE_ADD(CURDATE(), INTERVAL 89 DAY), 0, 0, 2, null, '109.99', '190711193001', ''),</v>
-      </c>
-    </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1193, 1193, 1, DATE_ADD(CURDATE(), INTERVAL 85 DAY), DATE_ADD(CURDATE(), INTERVAL 89 DAY), 0, 0, 2, null, '109.99', '190711193001', '', 1),</v>
+      </c>
+    </row>
+    <row r="195" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A195" s="6">
         <v>1194</v>
       </c>
@@ -24086,12 +24672,15 @@
       <c r="L195" s="11" t="s">
         <v>1479</v>
       </c>
-      <c r="M195" s="11" t="str">
-        <f t="shared" ref="M195:M200" si="3">"("&amp;A195&amp;", "&amp;B195&amp;", "&amp;C195&amp;", "&amp;D195&amp;", "&amp;E195&amp;", "&amp;F195&amp;", "&amp;G195&amp;", "&amp;H195&amp;", "&amp;I195&amp;", '"&amp;J195&amp;"', '"&amp;K195&amp;"', '"&amp;L195&amp;"'),"</f>
-        <v>(1194, 1194, 2, DATE_ADD(CURDATE(), INTERVAL 95 DAY), DATE_ADD(CURDATE(), INTERVAL 96 DAY), 0, 0, 1, null, '119.99', '190712194001', 'wants a large screen tv'),</v>
-      </c>
-    </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M195" s="6">
+        <v>1</v>
+      </c>
+      <c r="N195" s="11" t="str">
+        <f t="shared" ref="N195:N201" si="3">"("&amp;A195&amp;", "&amp;B195&amp;", "&amp;C195&amp;", "&amp;D195&amp;", "&amp;E195&amp;", "&amp;F195&amp;", "&amp;G195&amp;", "&amp;H195&amp;", "&amp;I195&amp;", '"&amp;J195&amp;"', '"&amp;K195&amp;"', '"&amp;L195&amp;"', "&amp;M195&amp;"),"</f>
+        <v>(1194, 1194, 2, DATE_ADD(CURDATE(), INTERVAL 95 DAY), DATE_ADD(CURDATE(), INTERVAL 96 DAY), 0, 0, 1, null, '119.99', '190712194001', 'wants a large screen tv', 1),</v>
+      </c>
+    </row>
+    <row r="196" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A196" s="6">
         <v>1195</v>
       </c>
@@ -24126,12 +24715,15 @@
         <v>1675</v>
       </c>
       <c r="L196" s="11"/>
-      <c r="M196" s="11" t="str">
+      <c r="M196" s="6">
+        <v>1</v>
+      </c>
+      <c r="N196" s="11" t="str">
         <f t="shared" si="3"/>
-        <v>(1195, 1195, 1, DATE_ADD(CURDATE(), INTERVAL 98 DAY), DATE_ADD(CURDATE(), INTERVAL 100 DAY), 0, 0, 3, null, '109.99', '190712195001', ''),</v>
-      </c>
-    </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1195, 1195, 1, DATE_ADD(CURDATE(), INTERVAL 98 DAY), DATE_ADD(CURDATE(), INTERVAL 100 DAY), 0, 0, 3, null, '109.99', '190712195001', '', 1),</v>
+      </c>
+    </row>
+    <row r="197" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A197" s="6">
         <v>1196</v>
       </c>
@@ -24166,12 +24758,15 @@
         <v>1676</v>
       </c>
       <c r="L197" s="11"/>
-      <c r="M197" s="11" t="str">
+      <c r="M197" s="6">
+        <v>1</v>
+      </c>
+      <c r="N197" s="11" t="str">
         <f t="shared" si="3"/>
-        <v>(1196, 1196, 3, DATE_ADD(CURDATE(), INTERVAL 101 DAY), DATE_ADD(CURDATE(), INTERVAL 102 DAY), 0, 0, 2, null, '129.99', '190713196001', ''),</v>
-      </c>
-    </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1196, 1196, 3, DATE_ADD(CURDATE(), INTERVAL 101 DAY), DATE_ADD(CURDATE(), INTERVAL 102 DAY), 0, 0, 2, null, '129.99', '190713196001', '', 1),</v>
+      </c>
+    </row>
+    <row r="198" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A198" s="6">
         <v>1197</v>
       </c>
@@ -24208,12 +24803,15 @@
       <c r="L198" s="11" t="s">
         <v>1478</v>
       </c>
-      <c r="M198" s="11" t="str">
+      <c r="M198" s="6">
+        <v>1</v>
+      </c>
+      <c r="N198" s="11" t="str">
         <f t="shared" si="3"/>
-        <v>(1197, 1197, 1, DATE_ADD(CURDATE(), INTERVAL 106 DAY), DATE_ADD(CURDATE(), INTERVAL 107 DAY), 0, 0, 2, null, '109.99', '190713197001', 'needs a late checkout time'),</v>
-      </c>
-    </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1197, 1197, 1, DATE_ADD(CURDATE(), INTERVAL 106 DAY), DATE_ADD(CURDATE(), INTERVAL 107 DAY), 0, 0, 2, null, '109.99', '190713197001', 'needs a late checkout time', 1),</v>
+      </c>
+    </row>
+    <row r="199" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A199" s="6">
         <v>1198</v>
       </c>
@@ -24248,12 +24846,15 @@
         <v>1678</v>
       </c>
       <c r="L199" s="11"/>
-      <c r="M199" s="11" t="str">
+      <c r="M199" s="6">
+        <v>1</v>
+      </c>
+      <c r="N199" s="11" t="str">
         <f t="shared" si="3"/>
-        <v>(1198, 1198, 3, DATE_ADD(CURDATE(), INTERVAL 108 DAY), DATE_ADD(CURDATE(), INTERVAL 110 DAY), 0, 0, 2, null, '129.99', '190713198001', ''),</v>
-      </c>
-    </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1198, 1198, 3, DATE_ADD(CURDATE(), INTERVAL 108 DAY), DATE_ADD(CURDATE(), INTERVAL 110 DAY), 0, 0, 2, null, '129.99', '190713198001', '', 1),</v>
+      </c>
+    </row>
+    <row r="200" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A200" s="6">
         <v>1199</v>
       </c>
@@ -24288,12 +24889,15 @@
         <v>1679</v>
       </c>
       <c r="L200" s="11"/>
-      <c r="M200" s="11" t="str">
+      <c r="M200" s="6">
+        <v>1</v>
+      </c>
+      <c r="N200" s="11" t="str">
         <f t="shared" si="3"/>
-        <v>(1199, 1199, 1, DATE_ADD(CURDATE(), INTERVAL 111 DAY), DATE_ADD(CURDATE(), INTERVAL 116 DAY), 0, 0, 1, null, '109.99', '190714199001', ''),</v>
-      </c>
-    </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.3">
+        <v>(1199, 1199, 1, DATE_ADD(CURDATE(), INTERVAL 111 DAY), DATE_ADD(CURDATE(), INTERVAL 116 DAY), 0, 0, 1, null, '109.99', '190714199001', '', 1),</v>
+      </c>
+    </row>
+    <row r="201" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A201" s="6">
         <v>1200</v>
       </c>
@@ -24328,13 +24932,16 @@
         <v>1680</v>
       </c>
       <c r="L201" s="11"/>
-      <c r="M201" s="11" t="str">
-        <f>"("&amp;A201&amp;", "&amp;B201&amp;", "&amp;C201&amp;", "&amp;D201&amp;", "&amp;E201&amp;", "&amp;F201&amp;", "&amp;G201&amp;", "&amp;H201&amp;", "&amp;I201&amp;", '"&amp;J201&amp;"', '"&amp;K201&amp;"', '"&amp;L201&amp;"');"</f>
-        <v>(1200, 1200, 3, DATE_ADD(CURDATE(), INTERVAL 120 DAY), DATE_ADD(CURDATE(), INTERVAL 123 DAY), 0, 0, 3, null, '129.99', '190714200001', '');</v>
+      <c r="M201" s="6">
+        <v>1</v>
+      </c>
+      <c r="N201" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>(1200, 1200, 3, DATE_ADD(CURDATE(), INTERVAL 120 DAY), DATE_ADD(CURDATE(), INTERVAL 123 DAY), 0, 0, 3, null, '129.99', '190714200001', '', 1),</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M201">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N201">
     <sortCondition ref="A2:A201"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28190,7 +28797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117D2267-72D7-482F-A136-70E06D3C8037}">
   <dimension ref="A1:M201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M2" sqref="M2:M201"/>
     </sheetView>

</xml_diff>